<commit_message>
Added to LZ compression codewords compression to minimize encoded file size. Also added GZip compression for benchmark reason.
</commit_message>
<xml_diff>
--- a/StreamCompress/CompressionTests.xlsx
+++ b/StreamCompress/CompressionTests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Users\Kalle\Documents\Source\Opiskelu\high-speed-image-stream-compress\StreamCompress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C3140D-3B31-4FDA-BC10-52058210414C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B87289FD-72BB-4966-9A18-11995EF7E4E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2115" yWindow="3675" windowWidth="33990" windowHeight="18930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="33990" windowHeight="18930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestsAndResult" sheetId="1" r:id="rId1"/>
@@ -408,7 +408,7 @@
   <dimension ref="A1:O42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,6 +422,8 @@
     <col min="7" max="9" width="7.28515625" customWidth="1"/>
     <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" customWidth="1"/>
     <col min="14" max="14" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -516,12 +518,13 @@
         <v>2764854</v>
       </c>
       <c r="K7">
-        <v>3297060</v>
+        <v>2060668</v>
       </c>
       <c r="L7" s="1">
         <f>K7/J7</f>
-        <v>1.1924897300182939</v>
-      </c>
+        <v>0.74530807051656256</v>
+      </c>
+      <c r="M7" s="1"/>
       <c r="N7" t="str">
         <f>"--destination-file-suffix "&amp;D7&amp;"-crop"&amp;E7&amp;".enc --method "&amp;D7&amp;" --crop-left-px "&amp;F7&amp;" --crop-right-px "&amp;F7&amp;" --crop-top-px "&amp;F7&amp;" --crop-bottom-px "&amp;F7&amp;""</f>
         <v>--destination-file-suffix AsLZ78Encoded-crop0.enc --method AsLZ78Encoded --crop-left-px 0 --crop-right-px 0 --crop-top-px 0 --crop-bottom-px 0</v>
@@ -563,11 +566,11 @@
         <v>2393142</v>
       </c>
       <c r="K8">
-        <v>2936660</v>
+        <v>1835418</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" ref="L8:L42" si="5">K8/J8</f>
-        <v>1.2271148139140928</v>
+        <v>0.76694905693017801</v>
       </c>
       <c r="N8" t="str">
         <f t="shared" ref="N8:N42" si="6">"--destination-file-suffix "&amp;D8&amp;"-crop"&amp;E8&amp;".enc --method "&amp;D8&amp;" --crop-left-px "&amp;F8&amp;" --crop-right-px "&amp;F8&amp;" --crop-top-px "&amp;F8&amp;" --crop-bottom-px "&amp;F8&amp;""</f>
@@ -610,11 +613,11 @@
         <v>2046006</v>
       </c>
       <c r="K9">
-        <v>2581168</v>
+        <v>1613235</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" si="5"/>
-        <v>1.2615642378370346</v>
+        <v>0.7884800924337465</v>
       </c>
       <c r="N9" t="str">
         <f t="shared" si="6"/>
@@ -657,11 +660,11 @@
         <v>1723446</v>
       </c>
       <c r="K10">
-        <v>2253552</v>
+        <v>1408475</v>
       </c>
       <c r="L10" s="1">
         <f t="shared" si="5"/>
-        <v>1.3075849199800864</v>
+        <v>0.81724347615184922</v>
       </c>
       <c r="N10" t="str">
         <f t="shared" si="6"/>
@@ -704,11 +707,11 @@
         <v>1425462</v>
       </c>
       <c r="K11">
-        <v>1881468</v>
+        <v>1117127</v>
       </c>
       <c r="L11" s="1">
         <f t="shared" si="5"/>
-        <v>1.3199004954183275</v>
+        <v>0.78369468986195356</v>
       </c>
       <c r="N11" t="str">
         <f t="shared" si="6"/>
@@ -751,11 +754,11 @@
         <v>1152054</v>
       </c>
       <c r="K12">
-        <v>1512392</v>
+        <v>897988</v>
       </c>
       <c r="L12" s="1">
         <f t="shared" si="5"/>
-        <v>1.3127787412742806</v>
+        <v>0.77946693470965767</v>
       </c>
       <c r="N12" t="str">
         <f t="shared" si="6"/>
@@ -798,11 +801,11 @@
         <v>903222</v>
       </c>
       <c r="K13">
-        <v>1183608</v>
+        <v>702773</v>
       </c>
       <c r="L13" s="1">
         <f t="shared" si="5"/>
-        <v>1.3104286653779469</v>
+        <v>0.77807338616641308</v>
       </c>
       <c r="N13" t="str">
         <f t="shared" si="6"/>
@@ -845,11 +848,11 @@
         <v>678966</v>
       </c>
       <c r="K14">
-        <v>899424</v>
+        <v>505931</v>
       </c>
       <c r="L14" s="1">
         <f t="shared" si="5"/>
-        <v>1.3246966711146066</v>
+        <v>0.74514924164096585</v>
       </c>
       <c r="N14" t="str">
         <f t="shared" si="6"/>
@@ -892,11 +895,11 @@
         <v>479286</v>
       </c>
       <c r="K15">
-        <v>646044</v>
+        <v>363405</v>
       </c>
       <c r="L15" s="1">
         <f t="shared" si="5"/>
-        <v>1.3479300459433408</v>
+        <v>0.75822160463689736</v>
       </c>
       <c r="N15" t="str">
         <f t="shared" si="6"/>
@@ -939,11 +942,11 @@
         <v>304182</v>
       </c>
       <c r="K16">
-        <v>422100</v>
+        <v>224246</v>
       </c>
       <c r="L16" s="1">
         <f t="shared" si="5"/>
-        <v>1.3876560743239246</v>
+        <v>0.73720995982668269</v>
       </c>
       <c r="N16" t="str">
         <f t="shared" si="6"/>
@@ -986,11 +989,11 @@
         <v>153654</v>
       </c>
       <c r="K17">
-        <v>235756</v>
+        <v>117883</v>
       </c>
       <c r="L17" s="1">
         <f t="shared" si="5"/>
-        <v>1.534330378642925</v>
+        <v>0.76719772996472591</v>
       </c>
       <c r="N17" t="str">
         <f t="shared" si="6"/>
@@ -1033,11 +1036,11 @@
         <v>27702</v>
       </c>
       <c r="K18">
-        <v>53084</v>
+        <v>23230</v>
       </c>
       <c r="L18" s="1">
         <f t="shared" si="5"/>
-        <v>1.9162515341852573</v>
+        <v>0.83856761244675471</v>
       </c>
       <c r="N18" t="str">
         <f t="shared" si="6"/>
@@ -1079,11 +1082,11 @@
         <v>921654</v>
       </c>
       <c r="K19">
-        <v>1167992</v>
+        <v>693501</v>
       </c>
       <c r="L19" s="1">
         <f t="shared" si="5"/>
-        <v>1.2672781759749321</v>
+        <v>0.75245265576886766</v>
       </c>
       <c r="N19" t="str">
         <f t="shared" si="6"/>
@@ -1126,11 +1129,11 @@
         <v>797750</v>
       </c>
       <c r="K20">
-        <v>1047952</v>
+        <v>622227</v>
       </c>
       <c r="L20" s="1">
         <f t="shared" si="5"/>
-        <v>1.3136345973049202</v>
+        <v>0.77997743654026952</v>
       </c>
       <c r="N20" t="str">
         <f t="shared" si="6"/>
@@ -1173,11 +1176,11 @@
         <v>682038</v>
       </c>
       <c r="K21">
-        <v>924680</v>
+        <v>520138</v>
       </c>
       <c r="L21" s="1">
         <f t="shared" si="5"/>
-        <v>1.3557602362331718</v>
+        <v>0.76262319694797065</v>
       </c>
       <c r="N21" t="str">
         <f t="shared" si="6"/>
@@ -1220,11 +1223,11 @@
         <v>574518</v>
       </c>
       <c r="K22">
-        <v>802804</v>
+        <v>451583</v>
       </c>
       <c r="L22" s="1">
         <f t="shared" si="5"/>
-        <v>1.3973522152482603</v>
+        <v>0.78602062946678786</v>
       </c>
       <c r="N22" t="str">
         <f t="shared" si="6"/>
@@ -1267,11 +1270,11 @@
         <v>475190</v>
       </c>
       <c r="K23">
-        <v>669064</v>
+        <v>376354</v>
       </c>
       <c r="L23" s="1">
         <f t="shared" si="5"/>
-        <v>1.4079925924367096</v>
+        <v>0.79200740756329047</v>
       </c>
       <c r="N23" t="str">
         <f t="shared" si="6"/>
@@ -1314,11 +1317,11 @@
         <v>384054</v>
       </c>
       <c r="K24">
-        <v>538480</v>
+        <v>302900</v>
       </c>
       <c r="L24" s="1">
         <f t="shared" si="5"/>
-        <v>1.402094497128008</v>
+        <v>0.78869117363704067</v>
       </c>
       <c r="N24" t="str">
         <f t="shared" si="6"/>
@@ -1361,11 +1364,11 @@
         <v>301110</v>
       </c>
       <c r="K25">
-        <v>429556</v>
+        <v>228207</v>
       </c>
       <c r="L25" s="1">
         <f t="shared" si="5"/>
-        <v>1.4265750058118296</v>
+        <v>0.75788582245690939</v>
       </c>
       <c r="N25" t="str">
         <f t="shared" si="6"/>
@@ -1408,11 +1411,11 @@
         <v>226358</v>
       </c>
       <c r="K26">
-        <v>337364</v>
+        <v>179230</v>
       </c>
       <c r="L26" s="1">
         <f t="shared" si="5"/>
-        <v>1.4904001625743291</v>
+        <v>0.7917988319387872</v>
       </c>
       <c r="N26" t="str">
         <f t="shared" si="6"/>
@@ -1455,11 +1458,11 @@
         <v>159798</v>
       </c>
       <c r="K27">
-        <v>252868</v>
+        <v>126439</v>
       </c>
       <c r="L27" s="1">
         <f t="shared" si="5"/>
-        <v>1.582422808796105</v>
+        <v>0.79124269390105006</v>
       </c>
       <c r="N27" t="str">
         <f t="shared" si="6"/>
@@ -1502,11 +1505,11 @@
         <v>101430</v>
       </c>
       <c r="K28">
-        <v>166580</v>
+        <v>83295</v>
       </c>
       <c r="L28" s="1">
         <f t="shared" si="5"/>
-        <v>1.6423148969732821</v>
+        <v>0.82120674356699197</v>
       </c>
       <c r="N28" t="str">
         <f t="shared" si="6"/>
@@ -1549,11 +1552,11 @@
         <v>51254</v>
       </c>
       <c r="K29">
-        <v>92116</v>
+        <v>43185</v>
       </c>
       <c r="L29" s="1">
         <f t="shared" si="5"/>
-        <v>1.797245093065907</v>
+        <v>0.84256838490654384</v>
       </c>
       <c r="N29" t="str">
         <f t="shared" si="6"/>
@@ -1596,11 +1599,11 @@
         <v>9270</v>
       </c>
       <c r="K30">
-        <v>22676</v>
+        <v>9218</v>
       </c>
       <c r="L30" s="1">
         <f t="shared" si="5"/>
-        <v>2.446170442286947</v>
+        <v>0.99439050701186626</v>
       </c>
       <c r="N30" t="str">
         <f t="shared" si="6"/>

</xml_diff>

<commit_message>
Benchmark result, test doc update, compression test results
</commit_message>
<xml_diff>
--- a/StreamCompress/CompressionTests.xlsx
+++ b/StreamCompress/CompressionTests.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Users\Kalle\Documents\Source\Opiskelu\high-speed-image-stream-compress\StreamCompress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B87289FD-72BB-4966-9A18-11995EF7E4E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D56D12-9487-4D40-B0C0-56FD5234446C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="33990" windowHeight="18930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestsAndResult" sheetId="1" r:id="rId1"/>
+    <sheet name="Taul1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="17">
   <si>
     <t>Crop</t>
   </si>
@@ -78,6 +79,12 @@
   </si>
   <si>
     <t>Output Lenght</t>
+  </si>
+  <si>
+    <t>AsGrayScaleAsGZipEncoded</t>
+  </si>
+  <si>
+    <t>AsGZipEncoded</t>
   </si>
 </sst>
 </file>
@@ -140,6 +147,1192 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fi-FI"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.19401217740069518"/>
+          <c:y val="1.6007261809892055E-2"/>
+          <c:w val="0.79760882075242401"/>
+          <c:h val="0.78747858956400729"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Taul1!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AsGrayScaleAsGZipEncoded</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Taul1!$H$2:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>921654</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>797750</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>682038</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>574518</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>475190</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>384054</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>301110</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>226358</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>159798</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>101430</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>51254</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9270</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Taul1!$I$2:$I$13</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.67653154003563154</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.69484926355374488</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.70782566367269861</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.71890697941578852</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.70919000820724343</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.68568742937191129</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.67528145860316824</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.68024545189478614</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.6963478892101278</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.69023957409050574</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.71098841066063134</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.83193096008629985</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2272-435C-B3CF-5707047EE9AE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Taul1!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AsGrayScaleAsHuffmanEncoded</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Taul1!$H$2:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>921654</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>797750</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>682038</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>574518</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>475190</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>384054</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>301110</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>226358</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>159798</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>101430</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>51254</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9270</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Taul1!$J$2:$J$13</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.95170747373743292</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95307427138827949</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.95125784780320155</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.95112076558088698</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.94104042593488924</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.92776536632869333</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.92196871575171868</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.92151812615414519</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9211504524462133</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.90891255052745734</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.90217348889842741</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.96677454153182307</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2272-435C-B3CF-5707047EE9AE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Taul1!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AsGrayScaleAsLZ78Encoded</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Taul1!$H$2:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>921654</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>797750</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>682038</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>574518</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>475190</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>384054</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>301110</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>226358</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>159798</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>101430</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>51254</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9270</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Taul1!$K$2:$K$13</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.75245265576886766</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.77997743654026952</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.76262319694797065</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.78602062946678786</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.79200740756329047</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.78869117363704067</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.75788582245690939</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7917988319387872</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.79124269390105006</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.82120674356699197</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.84256838490654384</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.99439050701186626</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-2272-435C-B3CF-5707047EE9AE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="470289040"/>
+        <c:axId val="587426536"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="470289040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fi-FI"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="587426536"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="587426536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fi-FI"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="470289040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fi-FI"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fi-FI"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>609598</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>190499</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Kaavio 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A18005F8-50CA-4023-B5CA-27C3FCA0CA27}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -405,10 +1598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O42"/>
+  <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="L31" activeCellId="2" sqref="D31:D66 J31:J66 L31:L66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,46 +1685,45 @@
         <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7">
-        <f>E7*16</f>
+        <f t="shared" ref="F7:F18" si="0">E7*16</f>
         <v>0</v>
       </c>
       <c r="G7">
-        <f>B$1-F7*2</f>
+        <f t="shared" ref="G7:G18" si="1">B$1-F7*2</f>
         <v>1280</v>
       </c>
       <c r="H7">
-        <f>B$2-F7*2</f>
+        <f t="shared" ref="H7:H18" si="2">B$2-F7*2</f>
         <v>720</v>
       </c>
       <c r="I7">
-        <f>G7*H7</f>
+        <f t="shared" ref="I7:I18" si="3">G7*H7</f>
         <v>921600</v>
       </c>
       <c r="J7">
-        <f>I7*C7/8+54</f>
+        <f t="shared" ref="J7:J18" si="4">I7*C7/8+54</f>
         <v>2764854</v>
       </c>
       <c r="K7">
-        <v>2060668</v>
+        <v>1663682</v>
       </c>
       <c r="L7" s="1">
-        <f>K7/J7</f>
-        <v>0.74530807051656256</v>
-      </c>
-      <c r="M7" s="1"/>
+        <f t="shared" ref="L7:L18" si="5">K7/J7</f>
+        <v>0.60172508204773201</v>
+      </c>
       <c r="N7" t="str">
-        <f>"--destination-file-suffix "&amp;D7&amp;"-crop"&amp;E7&amp;".enc --method "&amp;D7&amp;" --crop-left-px "&amp;F7&amp;" --crop-right-px "&amp;F7&amp;" --crop-top-px "&amp;F7&amp;" --crop-bottom-px "&amp;F7&amp;""</f>
-        <v>--destination-file-suffix AsLZ78Encoded-crop0.enc --method AsLZ78Encoded --crop-left-px 0 --crop-right-px 0 --crop-top-px 0 --crop-bottom-px 0</v>
+        <f t="shared" ref="N7:N18" si="6">"--destination-file-suffix "&amp;D7&amp;"-crop"&amp;E7&amp;".enc --method "&amp;D7&amp;" --crop-left-px "&amp;F7&amp;" --crop-right-px "&amp;F7&amp;" --crop-top-px "&amp;F7&amp;" --crop-bottom-px "&amp;F7&amp;""</f>
+        <v>--destination-file-suffix AsGZipEncoded-crop0.enc --method AsGZipEncoded --crop-left-px 0 --crop-right-px 0 --crop-top-px 0 --crop-bottom-px 0</v>
       </c>
       <c r="O7" t="str">
-        <f>B$3&amp;N7&amp;B$4</f>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsLZ78Encoded-crop0.enc --method AsLZ78Encoded --crop-left-px 0 --crop-right-px 0 --crop-top-px 0 --crop-bottom-px 0 &gt;&gt;%resultFile%</v>
+        <f t="shared" ref="O7:O18" si="7">B$3&amp;N7&amp;B$4</f>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGZipEncoded-crop0.enc --method AsGZipEncoded --crop-left-px 0 --crop-right-px 0 --crop-top-px 0 --crop-bottom-px 0 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -539,46 +1731,46 @@
         <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E8">
         <f>E7+2</f>
         <v>2</v>
       </c>
       <c r="F8">
-        <f t="shared" ref="F8:F42" si="0">E8*16</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="G8">
-        <f t="shared" ref="G8:G42" si="1">B$1-F8*2</f>
+        <f t="shared" si="1"/>
         <v>1216</v>
       </c>
       <c r="H8">
-        <f t="shared" ref="H8:H42" si="2">B$2-F8*2</f>
+        <f t="shared" si="2"/>
         <v>656</v>
       </c>
       <c r="I8">
-        <f t="shared" ref="I8:I42" si="3">G8*H8</f>
+        <f t="shared" si="3"/>
         <v>797696</v>
       </c>
       <c r="J8">
-        <f t="shared" ref="J8:J42" si="4">I8*C8/8+54</f>
+        <f t="shared" si="4"/>
         <v>2393142</v>
       </c>
       <c r="K8">
-        <v>1835418</v>
+        <v>1480577</v>
       </c>
       <c r="L8" s="1">
-        <f t="shared" ref="L8:L42" si="5">K8/J8</f>
-        <v>0.76694905693017801</v>
+        <f t="shared" si="5"/>
+        <v>0.61867494699436976</v>
       </c>
       <c r="N8" t="str">
-        <f t="shared" ref="N8:N42" si="6">"--destination-file-suffix "&amp;D8&amp;"-crop"&amp;E8&amp;".enc --method "&amp;D8&amp;" --crop-left-px "&amp;F8&amp;" --crop-right-px "&amp;F8&amp;" --crop-top-px "&amp;F8&amp;" --crop-bottom-px "&amp;F8&amp;""</f>
-        <v>--destination-file-suffix AsLZ78Encoded-crop2.enc --method AsLZ78Encoded --crop-left-px 32 --crop-right-px 32 --crop-top-px 32 --crop-bottom-px 32</v>
+        <f t="shared" ref="N8:N66" si="8">"--destination-file-suffix "&amp;D8&amp;"-crop"&amp;E8&amp;".enc --method "&amp;D8&amp;" --crop-left-px "&amp;F8&amp;" --crop-right-px "&amp;F8&amp;" --crop-top-px "&amp;F8&amp;" --crop-bottom-px "&amp;F8&amp;""</f>
+        <v>--destination-file-suffix AsGZipEncoded-crop2.enc --method AsGZipEncoded --crop-left-px 32 --crop-right-px 32 --crop-top-px 32 --crop-bottom-px 32</v>
       </c>
       <c r="O8" t="str">
-        <f t="shared" ref="O8:O42" si="7">B$3&amp;N8&amp;B$4</f>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsLZ78Encoded-crop2.enc --method AsLZ78Encoded --crop-left-px 32 --crop-right-px 32 --crop-top-px 32 --crop-bottom-px 32 &gt;&gt;%resultFile%</v>
+        <f t="shared" ref="O8:O66" si="9">B$3&amp;N8&amp;B$4</f>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGZipEncoded-crop2.enc --method AsGZipEncoded --crop-left-px 32 --crop-right-px 32 --crop-top-px 32 --crop-bottom-px 32 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -586,10 +1778,10 @@
         <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E9">
-        <f t="shared" ref="E9:E18" si="8">E8+2</f>
+        <f t="shared" ref="E9:E18" si="10">E8+2</f>
         <v>4</v>
       </c>
       <c r="F9">
@@ -613,19 +1805,19 @@
         <v>2046006</v>
       </c>
       <c r="K9">
-        <v>1613235</v>
+        <v>1293441</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" si="5"/>
-        <v>0.7884800924337465</v>
+        <v>0.63217849801026982</v>
       </c>
       <c r="N9" t="str">
-        <f t="shared" si="6"/>
-        <v>--destination-file-suffix AsLZ78Encoded-crop4.enc --method AsLZ78Encoded --crop-left-px 64 --crop-right-px 64 --crop-top-px 64 --crop-bottom-px 64</v>
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGZipEncoded-crop4.enc --method AsGZipEncoded --crop-left-px 64 --crop-right-px 64 --crop-top-px 64 --crop-bottom-px 64</v>
       </c>
       <c r="O9" t="str">
-        <f t="shared" si="7"/>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsLZ78Encoded-crop4.enc --method AsLZ78Encoded --crop-left-px 64 --crop-right-px 64 --crop-top-px 64 --crop-bottom-px 64 &gt;&gt;%resultFile%</v>
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGZipEncoded-crop4.enc --method AsGZipEncoded --crop-left-px 64 --crop-right-px 64 --crop-top-px 64 --crop-bottom-px 64 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -633,10 +1825,10 @@
         <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="F10">
@@ -660,19 +1852,19 @@
         <v>1723446</v>
       </c>
       <c r="K10">
-        <v>1408475</v>
+        <v>1113992</v>
       </c>
       <c r="L10" s="1">
         <f t="shared" si="5"/>
-        <v>0.81724347615184922</v>
+        <v>0.64637476311993525</v>
       </c>
       <c r="N10" t="str">
-        <f t="shared" si="6"/>
-        <v>--destination-file-suffix AsLZ78Encoded-crop6.enc --method AsLZ78Encoded --crop-left-px 96 --crop-right-px 96 --crop-top-px 96 --crop-bottom-px 96</v>
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGZipEncoded-crop6.enc --method AsGZipEncoded --crop-left-px 96 --crop-right-px 96 --crop-top-px 96 --crop-bottom-px 96</v>
       </c>
       <c r="O10" t="str">
-        <f t="shared" si="7"/>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsLZ78Encoded-crop6.enc --method AsLZ78Encoded --crop-left-px 96 --crop-right-px 96 --crop-top-px 96 --crop-bottom-px 96 &gt;&gt;%resultFile%</v>
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGZipEncoded-crop6.enc --method AsGZipEncoded --crop-left-px 96 --crop-right-px 96 --crop-top-px 96 --crop-bottom-px 96 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -680,10 +1872,10 @@
         <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="F11">
@@ -707,19 +1899,19 @@
         <v>1425462</v>
       </c>
       <c r="K11">
-        <v>1117127</v>
+        <v>914175</v>
       </c>
       <c r="L11" s="1">
         <f t="shared" si="5"/>
-        <v>0.78369468986195356</v>
+        <v>0.64131839361554355</v>
       </c>
       <c r="N11" t="str">
-        <f t="shared" si="6"/>
-        <v>--destination-file-suffix AsLZ78Encoded-crop8.enc --method AsLZ78Encoded --crop-left-px 128 --crop-right-px 128 --crop-top-px 128 --crop-bottom-px 128</v>
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGZipEncoded-crop8.enc --method AsGZipEncoded --crop-left-px 128 --crop-right-px 128 --crop-top-px 128 --crop-bottom-px 128</v>
       </c>
       <c r="O11" t="str">
-        <f t="shared" si="7"/>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsLZ78Encoded-crop8.enc --method AsLZ78Encoded --crop-left-px 128 --crop-right-px 128 --crop-top-px 128 --crop-bottom-px 128 &gt;&gt;%resultFile%</v>
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGZipEncoded-crop8.enc --method AsGZipEncoded --crop-left-px 128 --crop-right-px 128 --crop-top-px 128 --crop-bottom-px 128 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -727,10 +1919,10 @@
         <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>10</v>
       </c>
       <c r="F12">
@@ -754,19 +1946,19 @@
         <v>1152054</v>
       </c>
       <c r="K12">
-        <v>897988</v>
+        <v>707554</v>
       </c>
       <c r="L12" s="1">
         <f t="shared" si="5"/>
-        <v>0.77946693470965767</v>
+        <v>0.61416739145908095</v>
       </c>
       <c r="N12" t="str">
-        <f t="shared" si="6"/>
-        <v>--destination-file-suffix AsLZ78Encoded-crop10.enc --method AsLZ78Encoded --crop-left-px 160 --crop-right-px 160 --crop-top-px 160 --crop-bottom-px 160</v>
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGZipEncoded-crop10.enc --method AsGZipEncoded --crop-left-px 160 --crop-right-px 160 --crop-top-px 160 --crop-bottom-px 160</v>
       </c>
       <c r="O12" t="str">
-        <f t="shared" si="7"/>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsLZ78Encoded-crop10.enc --method AsLZ78Encoded --crop-left-px 160 --crop-right-px 160 --crop-top-px 160 --crop-bottom-px 160 &gt;&gt;%resultFile%</v>
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGZipEncoded-crop10.enc --method AsGZipEncoded --crop-left-px 160 --crop-right-px 160 --crop-top-px 160 --crop-bottom-px 160 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -774,10 +1966,10 @@
         <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
       <c r="F13">
@@ -801,19 +1993,19 @@
         <v>903222</v>
       </c>
       <c r="K13">
-        <v>702773</v>
+        <v>542568</v>
       </c>
       <c r="L13" s="1">
         <f t="shared" si="5"/>
-        <v>0.77807338616641308</v>
+        <v>0.60070281724758701</v>
       </c>
       <c r="N13" t="str">
-        <f t="shared" si="6"/>
-        <v>--destination-file-suffix AsLZ78Encoded-crop12.enc --method AsLZ78Encoded --crop-left-px 192 --crop-right-px 192 --crop-top-px 192 --crop-bottom-px 192</v>
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGZipEncoded-crop12.enc --method AsGZipEncoded --crop-left-px 192 --crop-right-px 192 --crop-top-px 192 --crop-bottom-px 192</v>
       </c>
       <c r="O13" t="str">
-        <f t="shared" si="7"/>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsLZ78Encoded-crop12.enc --method AsLZ78Encoded --crop-left-px 192 --crop-right-px 192 --crop-top-px 192 --crop-bottom-px 192 &gt;&gt;%resultFile%</v>
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGZipEncoded-crop12.enc --method AsGZipEncoded --crop-left-px 192 --crop-right-px 192 --crop-top-px 192 --crop-bottom-px 192 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -821,10 +2013,10 @@
         <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>14</v>
       </c>
       <c r="F14">
@@ -848,19 +2040,19 @@
         <v>678966</v>
       </c>
       <c r="K14">
-        <v>505931</v>
+        <v>408084</v>
       </c>
       <c r="L14" s="1">
         <f t="shared" si="5"/>
-        <v>0.74514924164096585</v>
+        <v>0.60103745990226309</v>
       </c>
       <c r="N14" t="str">
-        <f t="shared" si="6"/>
-        <v>--destination-file-suffix AsLZ78Encoded-crop14.enc --method AsLZ78Encoded --crop-left-px 224 --crop-right-px 224 --crop-top-px 224 --crop-bottom-px 224</v>
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGZipEncoded-crop14.enc --method AsGZipEncoded --crop-left-px 224 --crop-right-px 224 --crop-top-px 224 --crop-bottom-px 224</v>
       </c>
       <c r="O14" t="str">
-        <f t="shared" si="7"/>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsLZ78Encoded-crop14.enc --method AsLZ78Encoded --crop-left-px 224 --crop-right-px 224 --crop-top-px 224 --crop-bottom-px 224 &gt;&gt;%resultFile%</v>
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGZipEncoded-crop14.enc --method AsGZipEncoded --crop-left-px 224 --crop-right-px 224 --crop-top-px 224 --crop-bottom-px 224 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -868,10 +2060,10 @@
         <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>16</v>
       </c>
       <c r="F15">
@@ -895,19 +2087,19 @@
         <v>479286</v>
       </c>
       <c r="K15">
-        <v>363405</v>
+        <v>290375</v>
       </c>
       <c r="L15" s="1">
         <f t="shared" si="5"/>
-        <v>0.75822160463689736</v>
+        <v>0.60584911722854418</v>
       </c>
       <c r="N15" t="str">
-        <f t="shared" si="6"/>
-        <v>--destination-file-suffix AsLZ78Encoded-crop16.enc --method AsLZ78Encoded --crop-left-px 256 --crop-right-px 256 --crop-top-px 256 --crop-bottom-px 256</v>
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGZipEncoded-crop16.enc --method AsGZipEncoded --crop-left-px 256 --crop-right-px 256 --crop-top-px 256 --crop-bottom-px 256</v>
       </c>
       <c r="O15" t="str">
-        <f t="shared" si="7"/>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsLZ78Encoded-crop16.enc --method AsLZ78Encoded --crop-left-px 256 --crop-right-px 256 --crop-top-px 256 --crop-bottom-px 256 &gt;&gt;%resultFile%</v>
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGZipEncoded-crop16.enc --method AsGZipEncoded --crop-left-px 256 --crop-right-px 256 --crop-top-px 256 --crop-bottom-px 256 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -915,10 +2107,10 @@
         <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>18</v>
       </c>
       <c r="F16">
@@ -942,19 +2134,19 @@
         <v>304182</v>
       </c>
       <c r="K16">
-        <v>224246</v>
+        <v>182221</v>
       </c>
       <c r="L16" s="1">
         <f t="shared" si="5"/>
-        <v>0.73720995982668269</v>
+        <v>0.59905254091300608</v>
       </c>
       <c r="N16" t="str">
-        <f t="shared" si="6"/>
-        <v>--destination-file-suffix AsLZ78Encoded-crop18.enc --method AsLZ78Encoded --crop-left-px 288 --crop-right-px 288 --crop-top-px 288 --crop-bottom-px 288</v>
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGZipEncoded-crop18.enc --method AsGZipEncoded --crop-left-px 288 --crop-right-px 288 --crop-top-px 288 --crop-bottom-px 288</v>
       </c>
       <c r="O16" t="str">
-        <f t="shared" si="7"/>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsLZ78Encoded-crop18.enc --method AsLZ78Encoded --crop-left-px 288 --crop-right-px 288 --crop-top-px 288 --crop-bottom-px 288 &gt;&gt;%resultFile%</v>
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGZipEncoded-crop18.enc --method AsGZipEncoded --crop-left-px 288 --crop-right-px 288 --crop-top-px 288 --crop-bottom-px 288 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="17" spans="3:15" x14ac:dyDescent="0.25">
@@ -962,10 +2154,10 @@
         <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>20</v>
       </c>
       <c r="F17">
@@ -989,19 +2181,19 @@
         <v>153654</v>
       </c>
       <c r="K17">
-        <v>117883</v>
+        <v>92936</v>
       </c>
       <c r="L17" s="1">
         <f t="shared" si="5"/>
-        <v>0.76719772996472591</v>
+        <v>0.60483944446613824</v>
       </c>
       <c r="N17" t="str">
-        <f t="shared" si="6"/>
-        <v>--destination-file-suffix AsLZ78Encoded-crop20.enc --method AsLZ78Encoded --crop-left-px 320 --crop-right-px 320 --crop-top-px 320 --crop-bottom-px 320</v>
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGZipEncoded-crop20.enc --method AsGZipEncoded --crop-left-px 320 --crop-right-px 320 --crop-top-px 320 --crop-bottom-px 320</v>
       </c>
       <c r="O17" t="str">
-        <f t="shared" si="7"/>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsLZ78Encoded-crop20.enc --method AsLZ78Encoded --crop-left-px 320 --crop-right-px 320 --crop-top-px 320 --crop-bottom-px 320 &gt;&gt;%resultFile%</v>
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGZipEncoded-crop20.enc --method AsGZipEncoded --crop-left-px 320 --crop-right-px 320 --crop-top-px 320 --crop-bottom-px 320 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="18" spans="3:15" x14ac:dyDescent="0.25">
@@ -1009,10 +2201,10 @@
         <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E18">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>22</v>
       </c>
       <c r="F18">
@@ -1036,27 +2228,27 @@
         <v>27702</v>
       </c>
       <c r="K18">
-        <v>23230</v>
+        <v>16942</v>
       </c>
       <c r="L18" s="1">
         <f t="shared" si="5"/>
-        <v>0.83856761244675471</v>
+        <v>0.61158039130748687</v>
       </c>
       <c r="N18" t="str">
-        <f t="shared" si="6"/>
-        <v>--destination-file-suffix AsLZ78Encoded-crop22.enc --method AsLZ78Encoded --crop-left-px 352 --crop-right-px 352 --crop-top-px 352 --crop-bottom-px 352</v>
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGZipEncoded-crop22.enc --method AsGZipEncoded --crop-left-px 352 --crop-right-px 352 --crop-top-px 352 --crop-bottom-px 352</v>
       </c>
       <c r="O18" t="str">
-        <f t="shared" si="7"/>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsLZ78Encoded-crop22.enc --method AsLZ78Encoded --crop-left-px 352 --crop-right-px 352 --crop-top-px 352 --crop-bottom-px 352 &gt;&gt;%resultFile%</v>
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGZipEncoded-crop22.enc --method AsGZipEncoded --crop-left-px 352 --crop-right-px 352 --crop-top-px 352 --crop-bottom-px 352 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="19" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C19">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -1066,552 +2258,553 @@
         <v>0</v>
       </c>
       <c r="G19">
-        <f t="shared" si="1"/>
+        <f>B$1-F19*2</f>
         <v>1280</v>
       </c>
       <c r="H19">
-        <f t="shared" si="2"/>
+        <f>B$2-F19*2</f>
         <v>720</v>
       </c>
       <c r="I19">
-        <f t="shared" si="3"/>
+        <f>G19*H19</f>
         <v>921600</v>
       </c>
       <c r="J19">
-        <f t="shared" si="4"/>
-        <v>921654</v>
+        <f>I19*C19/8+54</f>
+        <v>2764854</v>
       </c>
       <c r="K19">
-        <v>693501</v>
+        <v>2060668</v>
       </c>
       <c r="L19" s="1">
-        <f t="shared" si="5"/>
-        <v>0.75245265576886766</v>
-      </c>
+        <f>K19/J19</f>
+        <v>0.74530807051656256</v>
+      </c>
+      <c r="M19" s="1"/>
       <c r="N19" t="str">
-        <f t="shared" si="6"/>
-        <v>--destination-file-suffix AsGrayScaleAsLZ78Encoded-crop0.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 0 --crop-right-px 0 --crop-top-px 0 --crop-bottom-px 0</v>
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsLZ78Encoded-crop0.enc --method AsLZ78Encoded --crop-left-px 0 --crop-right-px 0 --crop-top-px 0 --crop-bottom-px 0</v>
       </c>
       <c r="O19" t="str">
-        <f t="shared" si="7"/>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsLZ78Encoded-crop0.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 0 --crop-right-px 0 --crop-top-px 0 --crop-bottom-px 0 &gt;&gt;%resultFile%</v>
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsLZ78Encoded-crop0.enc --method AsLZ78Encoded --crop-left-px 0 --crop-right-px 0 --crop-top-px 0 --crop-bottom-px 0 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="20" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C20">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E20">
         <f>E19+2</f>
         <v>2</v>
       </c>
       <c r="F20">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F20:F42" si="11">E20*16</f>
         <v>32</v>
       </c>
       <c r="G20">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="G20:G42" si="12">B$1-F20*2</f>
         <v>1216</v>
       </c>
       <c r="H20">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="H20:H42" si="13">B$2-F20*2</f>
         <v>656</v>
       </c>
       <c r="I20">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="I20:I42" si="14">G20*H20</f>
         <v>797696</v>
       </c>
       <c r="J20">
-        <f t="shared" si="4"/>
-        <v>797750</v>
+        <f t="shared" ref="J20:J42" si="15">I20*C20/8+54</f>
+        <v>2393142</v>
       </c>
       <c r="K20">
-        <v>622227</v>
+        <v>1835418</v>
       </c>
       <c r="L20" s="1">
-        <f t="shared" si="5"/>
-        <v>0.77997743654026952</v>
+        <f t="shared" ref="L20:L66" si="16">K20/J20</f>
+        <v>0.76694905693017801</v>
       </c>
       <c r="N20" t="str">
-        <f t="shared" si="6"/>
-        <v>--destination-file-suffix AsGrayScaleAsLZ78Encoded-crop2.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 32 --crop-right-px 32 --crop-top-px 32 --crop-bottom-px 32</v>
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsLZ78Encoded-crop2.enc --method AsLZ78Encoded --crop-left-px 32 --crop-right-px 32 --crop-top-px 32 --crop-bottom-px 32</v>
       </c>
       <c r="O20" t="str">
-        <f t="shared" si="7"/>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsLZ78Encoded-crop2.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 32 --crop-right-px 32 --crop-top-px 32 --crop-bottom-px 32 &gt;&gt;%resultFile%</v>
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsLZ78Encoded-crop2.enc --method AsLZ78Encoded --crop-left-px 32 --crop-right-px 32 --crop-top-px 32 --crop-bottom-px 32 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="21" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C21">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D21" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E21">
-        <f t="shared" ref="E21:E30" si="9">E20+2</f>
+        <f t="shared" ref="E21:E30" si="17">E20+2</f>
         <v>4</v>
       </c>
       <c r="F21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>64</v>
       </c>
       <c r="G21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="12"/>
         <v>1152</v>
       </c>
       <c r="H21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="13"/>
         <v>592</v>
       </c>
       <c r="I21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>681984</v>
       </c>
       <c r="J21">
-        <f t="shared" si="4"/>
-        <v>682038</v>
+        <f t="shared" si="15"/>
+        <v>2046006</v>
       </c>
       <c r="K21">
-        <v>520138</v>
+        <v>1613235</v>
       </c>
       <c r="L21" s="1">
-        <f t="shared" si="5"/>
-        <v>0.76262319694797065</v>
+        <f t="shared" si="16"/>
+        <v>0.7884800924337465</v>
       </c>
       <c r="N21" t="str">
-        <f t="shared" si="6"/>
-        <v>--destination-file-suffix AsGrayScaleAsLZ78Encoded-crop4.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 64 --crop-right-px 64 --crop-top-px 64 --crop-bottom-px 64</v>
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsLZ78Encoded-crop4.enc --method AsLZ78Encoded --crop-left-px 64 --crop-right-px 64 --crop-top-px 64 --crop-bottom-px 64</v>
       </c>
       <c r="O21" t="str">
-        <f t="shared" si="7"/>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsLZ78Encoded-crop4.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 64 --crop-right-px 64 --crop-top-px 64 --crop-bottom-px 64 &gt;&gt;%resultFile%</v>
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsLZ78Encoded-crop4.enc --method AsLZ78Encoded --crop-left-px 64 --crop-right-px 64 --crop-top-px 64 --crop-bottom-px 64 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="22" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C22">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D22" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>6</v>
       </c>
       <c r="F22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>96</v>
       </c>
       <c r="G22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="12"/>
         <v>1088</v>
       </c>
       <c r="H22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="13"/>
         <v>528</v>
       </c>
       <c r="I22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>574464</v>
       </c>
       <c r="J22">
-        <f t="shared" si="4"/>
-        <v>574518</v>
+        <f t="shared" si="15"/>
+        <v>1723446</v>
       </c>
       <c r="K22">
-        <v>451583</v>
+        <v>1408475</v>
       </c>
       <c r="L22" s="1">
-        <f t="shared" si="5"/>
-        <v>0.78602062946678786</v>
+        <f t="shared" si="16"/>
+        <v>0.81724347615184922</v>
       </c>
       <c r="N22" t="str">
-        <f t="shared" si="6"/>
-        <v>--destination-file-suffix AsGrayScaleAsLZ78Encoded-crop6.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 96 --crop-right-px 96 --crop-top-px 96 --crop-bottom-px 96</v>
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsLZ78Encoded-crop6.enc --method AsLZ78Encoded --crop-left-px 96 --crop-right-px 96 --crop-top-px 96 --crop-bottom-px 96</v>
       </c>
       <c r="O22" t="str">
-        <f t="shared" si="7"/>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsLZ78Encoded-crop6.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 96 --crop-right-px 96 --crop-top-px 96 --crop-bottom-px 96 &gt;&gt;%resultFile%</v>
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsLZ78Encoded-crop6.enc --method AsLZ78Encoded --crop-left-px 96 --crop-right-px 96 --crop-top-px 96 --crop-bottom-px 96 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="23" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C23">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D23" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E23">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>8</v>
       </c>
       <c r="F23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>128</v>
       </c>
       <c r="G23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="12"/>
         <v>1024</v>
       </c>
       <c r="H23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="13"/>
         <v>464</v>
       </c>
       <c r="I23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>475136</v>
       </c>
       <c r="J23">
-        <f t="shared" si="4"/>
-        <v>475190</v>
+        <f t="shared" si="15"/>
+        <v>1425462</v>
       </c>
       <c r="K23">
-        <v>376354</v>
+        <v>1117127</v>
       </c>
       <c r="L23" s="1">
-        <f t="shared" si="5"/>
-        <v>0.79200740756329047</v>
+        <f t="shared" si="16"/>
+        <v>0.78369468986195356</v>
       </c>
       <c r="N23" t="str">
-        <f t="shared" si="6"/>
-        <v>--destination-file-suffix AsGrayScaleAsLZ78Encoded-crop8.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 128 --crop-right-px 128 --crop-top-px 128 --crop-bottom-px 128</v>
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsLZ78Encoded-crop8.enc --method AsLZ78Encoded --crop-left-px 128 --crop-right-px 128 --crop-top-px 128 --crop-bottom-px 128</v>
       </c>
       <c r="O23" t="str">
-        <f t="shared" si="7"/>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsLZ78Encoded-crop8.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 128 --crop-right-px 128 --crop-top-px 128 --crop-bottom-px 128 &gt;&gt;%resultFile%</v>
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsLZ78Encoded-crop8.enc --method AsLZ78Encoded --crop-left-px 128 --crop-right-px 128 --crop-top-px 128 --crop-bottom-px 128 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="24" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C24">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D24" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
       <c r="F24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>160</v>
       </c>
       <c r="G24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="12"/>
         <v>960</v>
       </c>
       <c r="H24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="13"/>
         <v>400</v>
       </c>
       <c r="I24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>384000</v>
       </c>
       <c r="J24">
-        <f t="shared" si="4"/>
-        <v>384054</v>
+        <f t="shared" si="15"/>
+        <v>1152054</v>
       </c>
       <c r="K24">
-        <v>302900</v>
+        <v>897988</v>
       </c>
       <c r="L24" s="1">
-        <f t="shared" si="5"/>
-        <v>0.78869117363704067</v>
+        <f t="shared" si="16"/>
+        <v>0.77946693470965767</v>
       </c>
       <c r="N24" t="str">
-        <f t="shared" si="6"/>
-        <v>--destination-file-suffix AsGrayScaleAsLZ78Encoded-crop10.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 160 --crop-right-px 160 --crop-top-px 160 --crop-bottom-px 160</v>
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsLZ78Encoded-crop10.enc --method AsLZ78Encoded --crop-left-px 160 --crop-right-px 160 --crop-top-px 160 --crop-bottom-px 160</v>
       </c>
       <c r="O24" t="str">
-        <f t="shared" si="7"/>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsLZ78Encoded-crop10.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 160 --crop-right-px 160 --crop-top-px 160 --crop-bottom-px 160 &gt;&gt;%resultFile%</v>
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsLZ78Encoded-crop10.enc --method AsLZ78Encoded --crop-left-px 160 --crop-right-px 160 --crop-top-px 160 --crop-bottom-px 160 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="25" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C25">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E25">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>12</v>
       </c>
       <c r="F25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>192</v>
       </c>
       <c r="G25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="12"/>
         <v>896</v>
       </c>
       <c r="H25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="13"/>
         <v>336</v>
       </c>
       <c r="I25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>301056</v>
       </c>
       <c r="J25">
-        <f t="shared" si="4"/>
-        <v>301110</v>
+        <f t="shared" si="15"/>
+        <v>903222</v>
       </c>
       <c r="K25">
-        <v>228207</v>
+        <v>702773</v>
       </c>
       <c r="L25" s="1">
-        <f t="shared" si="5"/>
-        <v>0.75788582245690939</v>
+        <f t="shared" si="16"/>
+        <v>0.77807338616641308</v>
       </c>
       <c r="N25" t="str">
-        <f t="shared" si="6"/>
-        <v>--destination-file-suffix AsGrayScaleAsLZ78Encoded-crop12.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 192 --crop-right-px 192 --crop-top-px 192 --crop-bottom-px 192</v>
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsLZ78Encoded-crop12.enc --method AsLZ78Encoded --crop-left-px 192 --crop-right-px 192 --crop-top-px 192 --crop-bottom-px 192</v>
       </c>
       <c r="O25" t="str">
-        <f t="shared" si="7"/>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsLZ78Encoded-crop12.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 192 --crop-right-px 192 --crop-top-px 192 --crop-bottom-px 192 &gt;&gt;%resultFile%</v>
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsLZ78Encoded-crop12.enc --method AsLZ78Encoded --crop-left-px 192 --crop-right-px 192 --crop-top-px 192 --crop-bottom-px 192 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="26" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C26">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E26">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>14</v>
       </c>
       <c r="F26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>224</v>
       </c>
       <c r="G26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="12"/>
         <v>832</v>
       </c>
       <c r="H26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="13"/>
         <v>272</v>
       </c>
       <c r="I26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>226304</v>
       </c>
       <c r="J26">
-        <f t="shared" si="4"/>
-        <v>226358</v>
+        <f t="shared" si="15"/>
+        <v>678966</v>
       </c>
       <c r="K26">
-        <v>179230</v>
+        <v>505931</v>
       </c>
       <c r="L26" s="1">
-        <f t="shared" si="5"/>
-        <v>0.7917988319387872</v>
+        <f t="shared" si="16"/>
+        <v>0.74514924164096585</v>
       </c>
       <c r="N26" t="str">
-        <f t="shared" si="6"/>
-        <v>--destination-file-suffix AsGrayScaleAsLZ78Encoded-crop14.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 224 --crop-right-px 224 --crop-top-px 224 --crop-bottom-px 224</v>
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsLZ78Encoded-crop14.enc --method AsLZ78Encoded --crop-left-px 224 --crop-right-px 224 --crop-top-px 224 --crop-bottom-px 224</v>
       </c>
       <c r="O26" t="str">
-        <f t="shared" si="7"/>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsLZ78Encoded-crop14.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 224 --crop-right-px 224 --crop-top-px 224 --crop-bottom-px 224 &gt;&gt;%resultFile%</v>
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsLZ78Encoded-crop14.enc --method AsLZ78Encoded --crop-left-px 224 --crop-right-px 224 --crop-top-px 224 --crop-bottom-px 224 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="27" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C27">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D27" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E27">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>16</v>
       </c>
       <c r="F27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>256</v>
       </c>
       <c r="G27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="12"/>
         <v>768</v>
       </c>
       <c r="H27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="13"/>
         <v>208</v>
       </c>
       <c r="I27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>159744</v>
       </c>
       <c r="J27">
-        <f t="shared" si="4"/>
-        <v>159798</v>
+        <f t="shared" si="15"/>
+        <v>479286</v>
       </c>
       <c r="K27">
-        <v>126439</v>
+        <v>363405</v>
       </c>
       <c r="L27" s="1">
-        <f t="shared" si="5"/>
-        <v>0.79124269390105006</v>
+        <f t="shared" si="16"/>
+        <v>0.75822160463689736</v>
       </c>
       <c r="N27" t="str">
-        <f t="shared" si="6"/>
-        <v>--destination-file-suffix AsGrayScaleAsLZ78Encoded-crop16.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 256 --crop-right-px 256 --crop-top-px 256 --crop-bottom-px 256</v>
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsLZ78Encoded-crop16.enc --method AsLZ78Encoded --crop-left-px 256 --crop-right-px 256 --crop-top-px 256 --crop-bottom-px 256</v>
       </c>
       <c r="O27" t="str">
-        <f t="shared" si="7"/>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsLZ78Encoded-crop16.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 256 --crop-right-px 256 --crop-top-px 256 --crop-bottom-px 256 &gt;&gt;%resultFile%</v>
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsLZ78Encoded-crop16.enc --method AsLZ78Encoded --crop-left-px 256 --crop-right-px 256 --crop-top-px 256 --crop-bottom-px 256 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="28" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C28">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D28" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E28">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>18</v>
       </c>
       <c r="F28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>288</v>
       </c>
       <c r="G28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="12"/>
         <v>704</v>
       </c>
       <c r="H28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="13"/>
         <v>144</v>
       </c>
       <c r="I28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>101376</v>
       </c>
       <c r="J28">
-        <f t="shared" si="4"/>
-        <v>101430</v>
+        <f t="shared" si="15"/>
+        <v>304182</v>
       </c>
       <c r="K28">
-        <v>83295</v>
+        <v>224246</v>
       </c>
       <c r="L28" s="1">
-        <f t="shared" si="5"/>
-        <v>0.82120674356699197</v>
+        <f t="shared" si="16"/>
+        <v>0.73720995982668269</v>
       </c>
       <c r="N28" t="str">
-        <f t="shared" si="6"/>
-        <v>--destination-file-suffix AsGrayScaleAsLZ78Encoded-crop18.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 288 --crop-right-px 288 --crop-top-px 288 --crop-bottom-px 288</v>
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsLZ78Encoded-crop18.enc --method AsLZ78Encoded --crop-left-px 288 --crop-right-px 288 --crop-top-px 288 --crop-bottom-px 288</v>
       </c>
       <c r="O28" t="str">
-        <f t="shared" si="7"/>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsLZ78Encoded-crop18.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 288 --crop-right-px 288 --crop-top-px 288 --crop-bottom-px 288 &gt;&gt;%resultFile%</v>
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsLZ78Encoded-crop18.enc --method AsLZ78Encoded --crop-left-px 288 --crop-right-px 288 --crop-top-px 288 --crop-bottom-px 288 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="29" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C29">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D29" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E29">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>20</v>
       </c>
       <c r="F29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>320</v>
       </c>
       <c r="G29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="12"/>
         <v>640</v>
       </c>
       <c r="H29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="13"/>
         <v>80</v>
       </c>
       <c r="I29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>51200</v>
       </c>
       <c r="J29">
-        <f t="shared" si="4"/>
-        <v>51254</v>
+        <f t="shared" si="15"/>
+        <v>153654</v>
       </c>
       <c r="K29">
-        <v>43185</v>
+        <v>117883</v>
       </c>
       <c r="L29" s="1">
-        <f t="shared" si="5"/>
-        <v>0.84256838490654384</v>
+        <f t="shared" si="16"/>
+        <v>0.76719772996472591</v>
       </c>
       <c r="N29" t="str">
-        <f t="shared" si="6"/>
-        <v>--destination-file-suffix AsGrayScaleAsLZ78Encoded-crop20.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 320 --crop-right-px 320 --crop-top-px 320 --crop-bottom-px 320</v>
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsLZ78Encoded-crop20.enc --method AsLZ78Encoded --crop-left-px 320 --crop-right-px 320 --crop-top-px 320 --crop-bottom-px 320</v>
       </c>
       <c r="O29" t="str">
-        <f t="shared" si="7"/>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsLZ78Encoded-crop20.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 320 --crop-right-px 320 --crop-top-px 320 --crop-bottom-px 320 &gt;&gt;%resultFile%</v>
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsLZ78Encoded-crop20.enc --method AsLZ78Encoded --crop-left-px 320 --crop-right-px 320 --crop-top-px 320 --crop-bottom-px 320 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="30" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C30">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D30" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E30">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>22</v>
       </c>
       <c r="F30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>352</v>
       </c>
       <c r="G30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="12"/>
         <v>576</v>
       </c>
       <c r="H30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="13"/>
         <v>16</v>
       </c>
       <c r="I30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>9216</v>
       </c>
       <c r="J30">
-        <f t="shared" si="4"/>
-        <v>9270</v>
+        <f t="shared" si="15"/>
+        <v>27702</v>
       </c>
       <c r="K30">
-        <v>9218</v>
+        <v>23230</v>
       </c>
       <c r="L30" s="1">
-        <f t="shared" si="5"/>
-        <v>0.99439050701186626</v>
+        <f t="shared" si="16"/>
+        <v>0.83856761244675471</v>
       </c>
       <c r="N30" t="str">
-        <f t="shared" si="6"/>
-        <v>--destination-file-suffix AsGrayScaleAsLZ78Encoded-crop22.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 352 --crop-right-px 352 --crop-top-px 352 --crop-bottom-px 352</v>
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsLZ78Encoded-crop22.enc --method AsLZ78Encoded --crop-left-px 352 --crop-right-px 352 --crop-top-px 352 --crop-bottom-px 352</v>
       </c>
       <c r="O30" t="str">
-        <f t="shared" si="7"/>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsLZ78Encoded-crop22.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 352 --crop-right-px 352 --crop-top-px 352 --crop-bottom-px 352 &gt;&gt;%resultFile%</v>
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsLZ78Encoded-crop22.enc --method AsLZ78Encoded --crop-left-px 352 --crop-right-px 352 --crop-top-px 352 --crop-bottom-px 352 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="31" spans="3:15" x14ac:dyDescent="0.25">
@@ -1619,45 +2812,45 @@
         <v>8</v>
       </c>
       <c r="D31" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E31">
         <v>0</v>
       </c>
       <c r="F31">
-        <f>E31*16</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="G31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="12"/>
         <v>1280</v>
       </c>
       <c r="H31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="13"/>
         <v>720</v>
       </c>
       <c r="I31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>921600</v>
       </c>
       <c r="J31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>921654</v>
       </c>
       <c r="K31">
-        <v>877145</v>
+        <v>623528</v>
       </c>
       <c r="L31" s="1">
-        <f t="shared" si="5"/>
-        <v>0.95170747373743292</v>
+        <f t="shared" si="16"/>
+        <v>0.67653154003563154</v>
       </c>
       <c r="N31" t="str">
-        <f t="shared" si="6"/>
-        <v>--destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop0.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 0 --crop-right-px 0 --crop-top-px 0 --crop-bottom-px 0</v>
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsGZipEncoded-crop0.enc --method AsGrayScaleAsGZipEncoded --crop-left-px 0 --crop-right-px 0 --crop-top-px 0 --crop-bottom-px 0</v>
       </c>
       <c r="O31" t="str">
-        <f t="shared" si="7"/>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop0.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 0 --crop-right-px 0 --crop-top-px 0 --crop-bottom-px 0 &gt;&gt;%resultFile%</v>
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsGZipEncoded-crop0.enc --method AsGrayScaleAsGZipEncoded --crop-left-px 0 --crop-right-px 0 --crop-top-px 0 --crop-bottom-px 0 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="32" spans="3:15" x14ac:dyDescent="0.25">
@@ -1665,46 +2858,46 @@
         <v>8</v>
       </c>
       <c r="D32" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E32">
         <f>E31+2</f>
         <v>2</v>
       </c>
       <c r="F32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>32</v>
       </c>
       <c r="G32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="12"/>
         <v>1216</v>
       </c>
       <c r="H32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="13"/>
         <v>656</v>
       </c>
       <c r="I32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>797696</v>
       </c>
       <c r="J32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>797750</v>
       </c>
       <c r="K32">
-        <v>760315</v>
+        <v>554316</v>
       </c>
       <c r="L32" s="1">
-        <f t="shared" si="5"/>
-        <v>0.95307427138827949</v>
+        <f t="shared" si="16"/>
+        <v>0.69484926355374488</v>
       </c>
       <c r="N32" t="str">
-        <f t="shared" si="6"/>
-        <v>--destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop2.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 32 --crop-right-px 32 --crop-top-px 32 --crop-bottom-px 32</v>
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsGZipEncoded-crop2.enc --method AsGrayScaleAsGZipEncoded --crop-left-px 32 --crop-right-px 32 --crop-top-px 32 --crop-bottom-px 32</v>
       </c>
       <c r="O32" t="str">
-        <f t="shared" si="7"/>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop2.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 32 --crop-right-px 32 --crop-top-px 32 --crop-bottom-px 32 &gt;&gt;%resultFile%</v>
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsGZipEncoded-crop2.enc --method AsGrayScaleAsGZipEncoded --crop-left-px 32 --crop-right-px 32 --crop-top-px 32 --crop-bottom-px 32 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="33" spans="3:15" x14ac:dyDescent="0.25">
@@ -1712,46 +2905,46 @@
         <v>8</v>
       </c>
       <c r="D33" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E33">
-        <f t="shared" ref="E33:E42" si="10">E32+2</f>
+        <f t="shared" ref="E33:E42" si="18">E32+2</f>
         <v>4</v>
       </c>
       <c r="F33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>64</v>
       </c>
       <c r="G33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="12"/>
         <v>1152</v>
       </c>
       <c r="H33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="13"/>
         <v>592</v>
       </c>
       <c r="I33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>681984</v>
       </c>
       <c r="J33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>682038</v>
       </c>
       <c r="K33">
-        <v>648794</v>
+        <v>482764</v>
       </c>
       <c r="L33" s="1">
-        <f t="shared" si="5"/>
-        <v>0.95125784780320155</v>
+        <f t="shared" si="16"/>
+        <v>0.70782566367269861</v>
       </c>
       <c r="N33" t="str">
-        <f t="shared" si="6"/>
-        <v>--destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop4.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 64 --crop-right-px 64 --crop-top-px 64 --crop-bottom-px 64</v>
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsGZipEncoded-crop4.enc --method AsGrayScaleAsGZipEncoded --crop-left-px 64 --crop-right-px 64 --crop-top-px 64 --crop-bottom-px 64</v>
       </c>
       <c r="O33" t="str">
-        <f t="shared" si="7"/>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop4.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 64 --crop-right-px 64 --crop-top-px 64 --crop-bottom-px 64 &gt;&gt;%resultFile%</v>
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsGZipEncoded-crop4.enc --method AsGrayScaleAsGZipEncoded --crop-left-px 64 --crop-right-px 64 --crop-top-px 64 --crop-bottom-px 64 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="34" spans="3:15" x14ac:dyDescent="0.25">
@@ -1759,46 +2952,46 @@
         <v>8</v>
       </c>
       <c r="D34" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>6</v>
       </c>
       <c r="F34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>96</v>
       </c>
       <c r="G34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="12"/>
         <v>1088</v>
       </c>
       <c r="H34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="13"/>
         <v>528</v>
       </c>
       <c r="I34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>574464</v>
       </c>
       <c r="J34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>574518</v>
       </c>
       <c r="K34">
-        <v>546436</v>
+        <v>413025</v>
       </c>
       <c r="L34" s="1">
-        <f t="shared" si="5"/>
-        <v>0.95112076558088698</v>
+        <f t="shared" si="16"/>
+        <v>0.71890697941578852</v>
       </c>
       <c r="N34" t="str">
-        <f t="shared" si="6"/>
-        <v>--destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop6.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 96 --crop-right-px 96 --crop-top-px 96 --crop-bottom-px 96</v>
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsGZipEncoded-crop6.enc --method AsGrayScaleAsGZipEncoded --crop-left-px 96 --crop-right-px 96 --crop-top-px 96 --crop-bottom-px 96</v>
       </c>
       <c r="O34" t="str">
-        <f t="shared" si="7"/>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop6.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 96 --crop-right-px 96 --crop-top-px 96 --crop-bottom-px 96 &gt;&gt;%resultFile%</v>
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsGZipEncoded-crop6.enc --method AsGrayScaleAsGZipEncoded --crop-left-px 96 --crop-right-px 96 --crop-top-px 96 --crop-bottom-px 96 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="35" spans="3:15" x14ac:dyDescent="0.25">
@@ -1806,46 +2999,46 @@
         <v>8</v>
       </c>
       <c r="D35" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>8</v>
       </c>
       <c r="F35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>128</v>
       </c>
       <c r="G35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="12"/>
         <v>1024</v>
       </c>
       <c r="H35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="13"/>
         <v>464</v>
       </c>
       <c r="I35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>475136</v>
       </c>
       <c r="J35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>475190</v>
       </c>
       <c r="K35">
-        <v>447173</v>
+        <v>337000</v>
       </c>
       <c r="L35" s="1">
-        <f t="shared" si="5"/>
-        <v>0.94104042593488924</v>
+        <f t="shared" si="16"/>
+        <v>0.70919000820724343</v>
       </c>
       <c r="N35" t="str">
-        <f t="shared" si="6"/>
-        <v>--destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop8.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 128 --crop-right-px 128 --crop-top-px 128 --crop-bottom-px 128</v>
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsGZipEncoded-crop8.enc --method AsGrayScaleAsGZipEncoded --crop-left-px 128 --crop-right-px 128 --crop-top-px 128 --crop-bottom-px 128</v>
       </c>
       <c r="O35" t="str">
-        <f t="shared" si="7"/>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop8.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 128 --crop-right-px 128 --crop-top-px 128 --crop-bottom-px 128 &gt;&gt;%resultFile%</v>
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsGZipEncoded-crop8.enc --method AsGrayScaleAsGZipEncoded --crop-left-px 128 --crop-right-px 128 --crop-top-px 128 --crop-bottom-px 128 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="36" spans="3:15" x14ac:dyDescent="0.25">
@@ -1853,46 +3046,46 @@
         <v>8</v>
       </c>
       <c r="D36" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E36">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>10</v>
       </c>
       <c r="F36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>160</v>
       </c>
       <c r="G36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="12"/>
         <v>960</v>
       </c>
       <c r="H36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="13"/>
         <v>400</v>
       </c>
       <c r="I36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>384000</v>
       </c>
       <c r="J36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>384054</v>
       </c>
       <c r="K36">
-        <v>356312</v>
+        <v>263341</v>
       </c>
       <c r="L36" s="1">
-        <f t="shared" si="5"/>
-        <v>0.92776536632869333</v>
+        <f t="shared" si="16"/>
+        <v>0.68568742937191129</v>
       </c>
       <c r="N36" t="str">
-        <f t="shared" si="6"/>
-        <v>--destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop10.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 160 --crop-right-px 160 --crop-top-px 160 --crop-bottom-px 160</v>
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsGZipEncoded-crop10.enc --method AsGrayScaleAsGZipEncoded --crop-left-px 160 --crop-right-px 160 --crop-top-px 160 --crop-bottom-px 160</v>
       </c>
       <c r="O36" t="str">
-        <f t="shared" si="7"/>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop10.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 160 --crop-right-px 160 --crop-top-px 160 --crop-bottom-px 160 &gt;&gt;%resultFile%</v>
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsGZipEncoded-crop10.enc --method AsGrayScaleAsGZipEncoded --crop-left-px 160 --crop-right-px 160 --crop-top-px 160 --crop-bottom-px 160 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="37" spans="3:15" x14ac:dyDescent="0.25">
@@ -1900,46 +3093,46 @@
         <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E37">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>12</v>
       </c>
       <c r="F37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>192</v>
       </c>
       <c r="G37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="12"/>
         <v>896</v>
       </c>
       <c r="H37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="13"/>
         <v>336</v>
       </c>
       <c r="I37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>301056</v>
       </c>
       <c r="J37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>301110</v>
       </c>
       <c r="K37">
-        <v>277614</v>
+        <v>203334</v>
       </c>
       <c r="L37" s="1">
-        <f t="shared" si="5"/>
-        <v>0.92196871575171868</v>
+        <f t="shared" si="16"/>
+        <v>0.67528145860316824</v>
       </c>
       <c r="N37" t="str">
-        <f t="shared" si="6"/>
-        <v>--destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop12.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 192 --crop-right-px 192 --crop-top-px 192 --crop-bottom-px 192</v>
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsGZipEncoded-crop12.enc --method AsGrayScaleAsGZipEncoded --crop-left-px 192 --crop-right-px 192 --crop-top-px 192 --crop-bottom-px 192</v>
       </c>
       <c r="O37" t="str">
-        <f t="shared" si="7"/>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop12.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 192 --crop-right-px 192 --crop-top-px 192 --crop-bottom-px 192 &gt;&gt;%resultFile%</v>
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsGZipEncoded-crop12.enc --method AsGrayScaleAsGZipEncoded --crop-left-px 192 --crop-right-px 192 --crop-top-px 192 --crop-bottom-px 192 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="38" spans="3:15" x14ac:dyDescent="0.25">
@@ -1947,46 +3140,46 @@
         <v>8</v>
       </c>
       <c r="D38" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>14</v>
       </c>
       <c r="F38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>224</v>
       </c>
       <c r="G38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="12"/>
         <v>832</v>
       </c>
       <c r="H38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="13"/>
         <v>272</v>
       </c>
       <c r="I38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>226304</v>
       </c>
       <c r="J38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>226358</v>
       </c>
       <c r="K38">
-        <v>208593</v>
+        <v>153979</v>
       </c>
       <c r="L38" s="1">
-        <f t="shared" si="5"/>
-        <v>0.92151812615414519</v>
+        <f t="shared" si="16"/>
+        <v>0.68024545189478614</v>
       </c>
       <c r="N38" t="str">
-        <f t="shared" si="6"/>
-        <v>--destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop14.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 224 --crop-right-px 224 --crop-top-px 224 --crop-bottom-px 224</v>
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsGZipEncoded-crop14.enc --method AsGrayScaleAsGZipEncoded --crop-left-px 224 --crop-right-px 224 --crop-top-px 224 --crop-bottom-px 224</v>
       </c>
       <c r="O38" t="str">
-        <f t="shared" si="7"/>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop14.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 224 --crop-right-px 224 --crop-top-px 224 --crop-bottom-px 224 &gt;&gt;%resultFile%</v>
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsGZipEncoded-crop14.enc --method AsGrayScaleAsGZipEncoded --crop-left-px 224 --crop-right-px 224 --crop-top-px 224 --crop-bottom-px 224 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="39" spans="3:15" x14ac:dyDescent="0.25">
@@ -1994,46 +3187,46 @@
         <v>8</v>
       </c>
       <c r="D39" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E39">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>16</v>
       </c>
       <c r="F39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>256</v>
       </c>
       <c r="G39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="12"/>
         <v>768</v>
       </c>
       <c r="H39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="13"/>
         <v>208</v>
       </c>
       <c r="I39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>159744</v>
       </c>
       <c r="J39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>159798</v>
       </c>
       <c r="K39">
-        <v>147198</v>
+        <v>111275</v>
       </c>
       <c r="L39" s="1">
-        <f t="shared" si="5"/>
-        <v>0.9211504524462133</v>
+        <f t="shared" si="16"/>
+        <v>0.6963478892101278</v>
       </c>
       <c r="N39" t="str">
-        <f t="shared" si="6"/>
-        <v>--destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop16.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 256 --crop-right-px 256 --crop-top-px 256 --crop-bottom-px 256</v>
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsGZipEncoded-crop16.enc --method AsGrayScaleAsGZipEncoded --crop-left-px 256 --crop-right-px 256 --crop-top-px 256 --crop-bottom-px 256</v>
       </c>
       <c r="O39" t="str">
-        <f t="shared" si="7"/>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop16.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 256 --crop-right-px 256 --crop-top-px 256 --crop-bottom-px 256 &gt;&gt;%resultFile%</v>
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsGZipEncoded-crop16.enc --method AsGrayScaleAsGZipEncoded --crop-left-px 256 --crop-right-px 256 --crop-top-px 256 --crop-bottom-px 256 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="40" spans="3:15" x14ac:dyDescent="0.25">
@@ -2041,46 +3234,46 @@
         <v>8</v>
       </c>
       <c r="D40" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>18</v>
       </c>
       <c r="F40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>288</v>
       </c>
       <c r="G40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="12"/>
         <v>704</v>
       </c>
       <c r="H40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="13"/>
         <v>144</v>
       </c>
       <c r="I40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>101376</v>
       </c>
       <c r="J40">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>101430</v>
       </c>
       <c r="K40">
-        <v>92191</v>
+        <v>70011</v>
       </c>
       <c r="L40" s="1">
-        <f t="shared" si="5"/>
-        <v>0.90891255052745734</v>
+        <f t="shared" si="16"/>
+        <v>0.69023957409050574</v>
       </c>
       <c r="N40" t="str">
-        <f t="shared" si="6"/>
-        <v>--destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop18.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 288 --crop-right-px 288 --crop-top-px 288 --crop-bottom-px 288</v>
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsGZipEncoded-crop18.enc --method AsGrayScaleAsGZipEncoded --crop-left-px 288 --crop-right-px 288 --crop-top-px 288 --crop-bottom-px 288</v>
       </c>
       <c r="O40" t="str">
-        <f t="shared" si="7"/>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop18.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 288 --crop-right-px 288 --crop-top-px 288 --crop-bottom-px 288 &gt;&gt;%resultFile%</v>
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsGZipEncoded-crop18.enc --method AsGrayScaleAsGZipEncoded --crop-left-px 288 --crop-right-px 288 --crop-top-px 288 --crop-bottom-px 288 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="41" spans="3:15" x14ac:dyDescent="0.25">
@@ -2088,46 +3281,46 @@
         <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E41">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>20</v>
       </c>
       <c r="F41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="11"/>
         <v>320</v>
       </c>
       <c r="G41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="12"/>
         <v>640</v>
       </c>
       <c r="H41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="13"/>
         <v>80</v>
       </c>
       <c r="I41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="14"/>
         <v>51200</v>
       </c>
       <c r="J41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="15"/>
         <v>51254</v>
       </c>
       <c r="K41">
-        <v>46240</v>
+        <v>36441</v>
       </c>
       <c r="L41" s="1">
-        <f t="shared" si="5"/>
-        <v>0.90217348889842741</v>
+        <f t="shared" si="16"/>
+        <v>0.71098841066063134</v>
       </c>
       <c r="N41" t="str">
-        <f t="shared" si="6"/>
-        <v>--destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop20.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 320 --crop-right-px 320 --crop-top-px 320 --crop-bottom-px 320</v>
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsGZipEncoded-crop20.enc --method AsGrayScaleAsGZipEncoded --crop-left-px 320 --crop-right-px 320 --crop-top-px 320 --crop-bottom-px 320</v>
       </c>
       <c r="O41" t="str">
-        <f t="shared" si="7"/>
-        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop20.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 320 --crop-right-px 320 --crop-top-px 320 --crop-bottom-px 320 &gt;&gt;%resultFile%</v>
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsGZipEncoded-crop20.enc --method AsGrayScaleAsGZipEncoded --crop-left-px 320 --crop-right-px 320 --crop-top-px 320 --crop-bottom-px 320 &gt;&gt;%resultFile%</v>
       </c>
     </row>
     <row r="42" spans="3:15" x14ac:dyDescent="0.25">
@@ -2135,45 +3328,1171 @@
         <v>8</v>
       </c>
       <c r="D42" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="18"/>
+        <v>22</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="11"/>
+        <v>352</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="12"/>
+        <v>576</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="13"/>
+        <v>16</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="14"/>
+        <v>9216</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="15"/>
+        <v>9270</v>
+      </c>
+      <c r="K42">
+        <v>7712</v>
+      </c>
+      <c r="L42" s="1">
+        <f t="shared" si="16"/>
+        <v>0.83193096008629985</v>
+      </c>
+      <c r="N42" t="str">
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsGZipEncoded-crop22.enc --method AsGrayScaleAsGZipEncoded --crop-left-px 352 --crop-right-px 352 --crop-top-px 352 --crop-bottom-px 352</v>
+      </c>
+      <c r="O42" t="str">
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsGZipEncoded-crop22.enc --method AsGrayScaleAsGZipEncoded --crop-left-px 352 --crop-right-px 352 --crop-top-px 352 --crop-bottom-px 352 &gt;&gt;%resultFile%</v>
+      </c>
+    </row>
+    <row r="43" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <v>8</v>
+      </c>
+      <c r="D43" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <f>E43*16</f>
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <f>B$1-F43*2</f>
+        <v>1280</v>
+      </c>
+      <c r="H43">
+        <f>B$2-F43*2</f>
+        <v>720</v>
+      </c>
+      <c r="I43">
+        <f>G43*H43</f>
+        <v>921600</v>
+      </c>
+      <c r="J43">
+        <f>I43*C43/8+54</f>
+        <v>921654</v>
+      </c>
+      <c r="K43">
+        <v>693501</v>
+      </c>
+      <c r="L43" s="1">
+        <f t="shared" si="16"/>
+        <v>0.75245265576886766</v>
+      </c>
+      <c r="N43" t="str">
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsLZ78Encoded-crop0.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 0 --crop-right-px 0 --crop-top-px 0 --crop-bottom-px 0</v>
+      </c>
+      <c r="O43" t="str">
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsLZ78Encoded-crop0.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 0 --crop-right-px 0 --crop-top-px 0 --crop-bottom-px 0 &gt;&gt;%resultFile%</v>
+      </c>
+    </row>
+    <row r="44" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <v>8</v>
+      </c>
+      <c r="D44" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44">
+        <f>E43+2</f>
+        <v>2</v>
+      </c>
+      <c r="F44">
+        <f>E44*16</f>
+        <v>32</v>
+      </c>
+      <c r="G44">
+        <f>B$1-F44*2</f>
+        <v>1216</v>
+      </c>
+      <c r="H44">
+        <f>B$2-F44*2</f>
+        <v>656</v>
+      </c>
+      <c r="I44">
+        <f>G44*H44</f>
+        <v>797696</v>
+      </c>
+      <c r="J44">
+        <f>I44*C44/8+54</f>
+        <v>797750</v>
+      </c>
+      <c r="K44">
+        <v>622227</v>
+      </c>
+      <c r="L44" s="1">
+        <f t="shared" si="16"/>
+        <v>0.77997743654026952</v>
+      </c>
+      <c r="N44" t="str">
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsLZ78Encoded-crop2.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 32 --crop-right-px 32 --crop-top-px 32 --crop-bottom-px 32</v>
+      </c>
+      <c r="O44" t="str">
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsLZ78Encoded-crop2.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 32 --crop-right-px 32 --crop-top-px 32 --crop-bottom-px 32 &gt;&gt;%resultFile%</v>
+      </c>
+    </row>
+    <row r="45" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <v>8</v>
+      </c>
+      <c r="D45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45">
+        <f t="shared" ref="E45:E54" si="19">E44+2</f>
+        <v>4</v>
+      </c>
+      <c r="F45">
+        <f>E45*16</f>
+        <v>64</v>
+      </c>
+      <c r="G45">
+        <f>B$1-F45*2</f>
+        <v>1152</v>
+      </c>
+      <c r="H45">
+        <f>B$2-F45*2</f>
+        <v>592</v>
+      </c>
+      <c r="I45">
+        <f>G45*H45</f>
+        <v>681984</v>
+      </c>
+      <c r="J45">
+        <f>I45*C45/8+54</f>
+        <v>682038</v>
+      </c>
+      <c r="K45">
+        <v>520138</v>
+      </c>
+      <c r="L45" s="1">
+        <f t="shared" si="16"/>
+        <v>0.76262319694797065</v>
+      </c>
+      <c r="N45" t="str">
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsLZ78Encoded-crop4.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 64 --crop-right-px 64 --crop-top-px 64 --crop-bottom-px 64</v>
+      </c>
+      <c r="O45" t="str">
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsLZ78Encoded-crop4.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 64 --crop-right-px 64 --crop-top-px 64 --crop-bottom-px 64 &gt;&gt;%resultFile%</v>
+      </c>
+    </row>
+    <row r="46" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <v>8</v>
+      </c>
+      <c r="D46" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="19"/>
+        <v>6</v>
+      </c>
+      <c r="F46">
+        <f>E46*16</f>
+        <v>96</v>
+      </c>
+      <c r="G46">
+        <f>B$1-F46*2</f>
+        <v>1088</v>
+      </c>
+      <c r="H46">
+        <f>B$2-F46*2</f>
+        <v>528</v>
+      </c>
+      <c r="I46">
+        <f>G46*H46</f>
+        <v>574464</v>
+      </c>
+      <c r="J46">
+        <f>I46*C46/8+54</f>
+        <v>574518</v>
+      </c>
+      <c r="K46">
+        <v>451583</v>
+      </c>
+      <c r="L46" s="1">
+        <f t="shared" si="16"/>
+        <v>0.78602062946678786</v>
+      </c>
+      <c r="N46" t="str">
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsLZ78Encoded-crop6.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 96 --crop-right-px 96 --crop-top-px 96 --crop-bottom-px 96</v>
+      </c>
+      <c r="O46" t="str">
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsLZ78Encoded-crop6.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 96 --crop-right-px 96 --crop-top-px 96 --crop-bottom-px 96 &gt;&gt;%resultFile%</v>
+      </c>
+    </row>
+    <row r="47" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C47">
+        <v>8</v>
+      </c>
+      <c r="D47" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="19"/>
+        <v>8</v>
+      </c>
+      <c r="F47">
+        <f>E47*16</f>
+        <v>128</v>
+      </c>
+      <c r="G47">
+        <f>B$1-F47*2</f>
+        <v>1024</v>
+      </c>
+      <c r="H47">
+        <f>B$2-F47*2</f>
+        <v>464</v>
+      </c>
+      <c r="I47">
+        <f>G47*H47</f>
+        <v>475136</v>
+      </c>
+      <c r="J47">
+        <f>I47*C47/8+54</f>
+        <v>475190</v>
+      </c>
+      <c r="K47">
+        <v>376354</v>
+      </c>
+      <c r="L47" s="1">
+        <f t="shared" si="16"/>
+        <v>0.79200740756329047</v>
+      </c>
+      <c r="N47" t="str">
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsLZ78Encoded-crop8.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 128 --crop-right-px 128 --crop-top-px 128 --crop-bottom-px 128</v>
+      </c>
+      <c r="O47" t="str">
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsLZ78Encoded-crop8.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 128 --crop-right-px 128 --crop-top-px 128 --crop-bottom-px 128 &gt;&gt;%resultFile%</v>
+      </c>
+    </row>
+    <row r="48" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C48">
+        <v>8</v>
+      </c>
+      <c r="D48" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="19"/>
+        <v>10</v>
+      </c>
+      <c r="F48">
+        <f>E48*16</f>
+        <v>160</v>
+      </c>
+      <c r="G48">
+        <f>B$1-F48*2</f>
+        <v>960</v>
+      </c>
+      <c r="H48">
+        <f>B$2-F48*2</f>
+        <v>400</v>
+      </c>
+      <c r="I48">
+        <f>G48*H48</f>
+        <v>384000</v>
+      </c>
+      <c r="J48">
+        <f>I48*C48/8+54</f>
+        <v>384054</v>
+      </c>
+      <c r="K48">
+        <v>302900</v>
+      </c>
+      <c r="L48" s="1">
+        <f t="shared" si="16"/>
+        <v>0.78869117363704067</v>
+      </c>
+      <c r="N48" t="str">
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsLZ78Encoded-crop10.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 160 --crop-right-px 160 --crop-top-px 160 --crop-bottom-px 160</v>
+      </c>
+      <c r="O48" t="str">
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsLZ78Encoded-crop10.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 160 --crop-right-px 160 --crop-top-px 160 --crop-bottom-px 160 &gt;&gt;%resultFile%</v>
+      </c>
+    </row>
+    <row r="49" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <v>8</v>
+      </c>
+      <c r="D49" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="19"/>
+        <v>12</v>
+      </c>
+      <c r="F49">
+        <f>E49*16</f>
+        <v>192</v>
+      </c>
+      <c r="G49">
+        <f>B$1-F49*2</f>
+        <v>896</v>
+      </c>
+      <c r="H49">
+        <f>B$2-F49*2</f>
+        <v>336</v>
+      </c>
+      <c r="I49">
+        <f>G49*H49</f>
+        <v>301056</v>
+      </c>
+      <c r="J49">
+        <f>I49*C49/8+54</f>
+        <v>301110</v>
+      </c>
+      <c r="K49">
+        <v>228207</v>
+      </c>
+      <c r="L49" s="1">
+        <f t="shared" si="16"/>
+        <v>0.75788582245690939</v>
+      </c>
+      <c r="N49" t="str">
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsLZ78Encoded-crop12.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 192 --crop-right-px 192 --crop-top-px 192 --crop-bottom-px 192</v>
+      </c>
+      <c r="O49" t="str">
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsLZ78Encoded-crop12.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 192 --crop-right-px 192 --crop-top-px 192 --crop-bottom-px 192 &gt;&gt;%resultFile%</v>
+      </c>
+    </row>
+    <row r="50" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C50">
+        <v>8</v>
+      </c>
+      <c r="D50" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="19"/>
+        <v>14</v>
+      </c>
+      <c r="F50">
+        <f>E50*16</f>
+        <v>224</v>
+      </c>
+      <c r="G50">
+        <f>B$1-F50*2</f>
+        <v>832</v>
+      </c>
+      <c r="H50">
+        <f>B$2-F50*2</f>
+        <v>272</v>
+      </c>
+      <c r="I50">
+        <f>G50*H50</f>
+        <v>226304</v>
+      </c>
+      <c r="J50">
+        <f>I50*C50/8+54</f>
+        <v>226358</v>
+      </c>
+      <c r="K50">
+        <v>179230</v>
+      </c>
+      <c r="L50" s="1">
+        <f t="shared" si="16"/>
+        <v>0.7917988319387872</v>
+      </c>
+      <c r="N50" t="str">
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsLZ78Encoded-crop14.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 224 --crop-right-px 224 --crop-top-px 224 --crop-bottom-px 224</v>
+      </c>
+      <c r="O50" t="str">
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsLZ78Encoded-crop14.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 224 --crop-right-px 224 --crop-top-px 224 --crop-bottom-px 224 &gt;&gt;%resultFile%</v>
+      </c>
+    </row>
+    <row r="51" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <v>8</v>
+      </c>
+      <c r="D51" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="19"/>
+        <v>16</v>
+      </c>
+      <c r="F51">
+        <f>E51*16</f>
+        <v>256</v>
+      </c>
+      <c r="G51">
+        <f>B$1-F51*2</f>
+        <v>768</v>
+      </c>
+      <c r="H51">
+        <f>B$2-F51*2</f>
+        <v>208</v>
+      </c>
+      <c r="I51">
+        <f>G51*H51</f>
+        <v>159744</v>
+      </c>
+      <c r="J51">
+        <f>I51*C51/8+54</f>
+        <v>159798</v>
+      </c>
+      <c r="K51">
+        <v>126439</v>
+      </c>
+      <c r="L51" s="1">
+        <f t="shared" si="16"/>
+        <v>0.79124269390105006</v>
+      </c>
+      <c r="N51" t="str">
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsLZ78Encoded-crop16.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 256 --crop-right-px 256 --crop-top-px 256 --crop-bottom-px 256</v>
+      </c>
+      <c r="O51" t="str">
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsLZ78Encoded-crop16.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 256 --crop-right-px 256 --crop-top-px 256 --crop-bottom-px 256 &gt;&gt;%resultFile%</v>
+      </c>
+    </row>
+    <row r="52" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C52">
+        <v>8</v>
+      </c>
+      <c r="D52" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="19"/>
+        <v>18</v>
+      </c>
+      <c r="F52">
+        <f>E52*16</f>
+        <v>288</v>
+      </c>
+      <c r="G52">
+        <f>B$1-F52*2</f>
+        <v>704</v>
+      </c>
+      <c r="H52">
+        <f>B$2-F52*2</f>
+        <v>144</v>
+      </c>
+      <c r="I52">
+        <f>G52*H52</f>
+        <v>101376</v>
+      </c>
+      <c r="J52">
+        <f>I52*C52/8+54</f>
+        <v>101430</v>
+      </c>
+      <c r="K52">
+        <v>83295</v>
+      </c>
+      <c r="L52" s="1">
+        <f t="shared" si="16"/>
+        <v>0.82120674356699197</v>
+      </c>
+      <c r="N52" t="str">
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsLZ78Encoded-crop18.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 288 --crop-right-px 288 --crop-top-px 288 --crop-bottom-px 288</v>
+      </c>
+      <c r="O52" t="str">
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsLZ78Encoded-crop18.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 288 --crop-right-px 288 --crop-top-px 288 --crop-bottom-px 288 &gt;&gt;%resultFile%</v>
+      </c>
+    </row>
+    <row r="53" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C53">
+        <v>8</v>
+      </c>
+      <c r="D53" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="19"/>
+        <v>20</v>
+      </c>
+      <c r="F53">
+        <f>E53*16</f>
+        <v>320</v>
+      </c>
+      <c r="G53">
+        <f>B$1-F53*2</f>
+        <v>640</v>
+      </c>
+      <c r="H53">
+        <f>B$2-F53*2</f>
+        <v>80</v>
+      </c>
+      <c r="I53">
+        <f>G53*H53</f>
+        <v>51200</v>
+      </c>
+      <c r="J53">
+        <f>I53*C53/8+54</f>
+        <v>51254</v>
+      </c>
+      <c r="K53">
+        <v>43185</v>
+      </c>
+      <c r="L53" s="1">
+        <f t="shared" si="16"/>
+        <v>0.84256838490654384</v>
+      </c>
+      <c r="N53" t="str">
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsLZ78Encoded-crop20.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 320 --crop-right-px 320 --crop-top-px 320 --crop-bottom-px 320</v>
+      </c>
+      <c r="O53" t="str">
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsLZ78Encoded-crop20.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 320 --crop-right-px 320 --crop-top-px 320 --crop-bottom-px 320 &gt;&gt;%resultFile%</v>
+      </c>
+    </row>
+    <row r="54" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C54">
+        <v>8</v>
+      </c>
+      <c r="D54" t="s">
+        <v>8</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="19"/>
+        <v>22</v>
+      </c>
+      <c r="F54">
+        <f>E54*16</f>
+        <v>352</v>
+      </c>
+      <c r="G54">
+        <f>B$1-F54*2</f>
+        <v>576</v>
+      </c>
+      <c r="H54">
+        <f>B$2-F54*2</f>
+        <v>16</v>
+      </c>
+      <c r="I54">
+        <f>G54*H54</f>
+        <v>9216</v>
+      </c>
+      <c r="J54">
+        <f>I54*C54/8+54</f>
+        <v>9270</v>
+      </c>
+      <c r="K54">
+        <v>9218</v>
+      </c>
+      <c r="L54" s="1">
+        <f t="shared" si="16"/>
+        <v>0.99439050701186626</v>
+      </c>
+      <c r="N54" t="str">
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsLZ78Encoded-crop22.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 352 --crop-right-px 352 --crop-top-px 352 --crop-bottom-px 352</v>
+      </c>
+      <c r="O54" t="str">
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsLZ78Encoded-crop22.enc --method AsGrayScaleAsLZ78Encoded --crop-left-px 352 --crop-right-px 352 --crop-top-px 352 --crop-bottom-px 352 &gt;&gt;%resultFile%</v>
+      </c>
+    </row>
+    <row r="55" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C55">
+        <v>8</v>
+      </c>
+      <c r="D55" t="s">
         <v>9</v>
       </c>
-      <c r="E42">
-        <f t="shared" si="10"/>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <f>E55*16</f>
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <f>B$1-F55*2</f>
+        <v>1280</v>
+      </c>
+      <c r="H55">
+        <f>B$2-F55*2</f>
+        <v>720</v>
+      </c>
+      <c r="I55">
+        <f>G55*H55</f>
+        <v>921600</v>
+      </c>
+      <c r="J55">
+        <f>I55*C55/8+54</f>
+        <v>921654</v>
+      </c>
+      <c r="K55">
+        <v>877145</v>
+      </c>
+      <c r="L55" s="1">
+        <f t="shared" si="16"/>
+        <v>0.95170747373743292</v>
+      </c>
+      <c r="N55" t="str">
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop0.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 0 --crop-right-px 0 --crop-top-px 0 --crop-bottom-px 0</v>
+      </c>
+      <c r="O55" t="str">
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop0.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 0 --crop-right-px 0 --crop-top-px 0 --crop-bottom-px 0 &gt;&gt;%resultFile%</v>
+      </c>
+    </row>
+    <row r="56" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C56">
+        <v>8</v>
+      </c>
+      <c r="D56" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56">
+        <f>E55+2</f>
+        <v>2</v>
+      </c>
+      <c r="F56">
+        <f>E56*16</f>
+        <v>32</v>
+      </c>
+      <c r="G56">
+        <f>B$1-F56*2</f>
+        <v>1216</v>
+      </c>
+      <c r="H56">
+        <f>B$2-F56*2</f>
+        <v>656</v>
+      </c>
+      <c r="I56">
+        <f>G56*H56</f>
+        <v>797696</v>
+      </c>
+      <c r="J56">
+        <f>I56*C56/8+54</f>
+        <v>797750</v>
+      </c>
+      <c r="K56">
+        <v>760315</v>
+      </c>
+      <c r="L56" s="1">
+        <f t="shared" si="16"/>
+        <v>0.95307427138827949</v>
+      </c>
+      <c r="N56" t="str">
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop2.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 32 --crop-right-px 32 --crop-top-px 32 --crop-bottom-px 32</v>
+      </c>
+      <c r="O56" t="str">
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop2.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 32 --crop-right-px 32 --crop-top-px 32 --crop-bottom-px 32 &gt;&gt;%resultFile%</v>
+      </c>
+    </row>
+    <row r="57" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C57">
+        <v>8</v>
+      </c>
+      <c r="D57" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57">
+        <f t="shared" ref="E57:E66" si="20">E56+2</f>
+        <v>4</v>
+      </c>
+      <c r="F57">
+        <f>E57*16</f>
+        <v>64</v>
+      </c>
+      <c r="G57">
+        <f>B$1-F57*2</f>
+        <v>1152</v>
+      </c>
+      <c r="H57">
+        <f>B$2-F57*2</f>
+        <v>592</v>
+      </c>
+      <c r="I57">
+        <f>G57*H57</f>
+        <v>681984</v>
+      </c>
+      <c r="J57">
+        <f>I57*C57/8+54</f>
+        <v>682038</v>
+      </c>
+      <c r="K57">
+        <v>648794</v>
+      </c>
+      <c r="L57" s="1">
+        <f t="shared" si="16"/>
+        <v>0.95125784780320155</v>
+      </c>
+      <c r="N57" t="str">
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop4.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 64 --crop-right-px 64 --crop-top-px 64 --crop-bottom-px 64</v>
+      </c>
+      <c r="O57" t="str">
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop4.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 64 --crop-right-px 64 --crop-top-px 64 --crop-bottom-px 64 &gt;&gt;%resultFile%</v>
+      </c>
+    </row>
+    <row r="58" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C58">
+        <v>8</v>
+      </c>
+      <c r="D58" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="20"/>
+        <v>6</v>
+      </c>
+      <c r="F58">
+        <f>E58*16</f>
+        <v>96</v>
+      </c>
+      <c r="G58">
+        <f>B$1-F58*2</f>
+        <v>1088</v>
+      </c>
+      <c r="H58">
+        <f>B$2-F58*2</f>
+        <v>528</v>
+      </c>
+      <c r="I58">
+        <f>G58*H58</f>
+        <v>574464</v>
+      </c>
+      <c r="J58">
+        <f>I58*C58/8+54</f>
+        <v>574518</v>
+      </c>
+      <c r="K58">
+        <v>546436</v>
+      </c>
+      <c r="L58" s="1">
+        <f t="shared" si="16"/>
+        <v>0.95112076558088698</v>
+      </c>
+      <c r="N58" t="str">
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop6.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 96 --crop-right-px 96 --crop-top-px 96 --crop-bottom-px 96</v>
+      </c>
+      <c r="O58" t="str">
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop6.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 96 --crop-right-px 96 --crop-top-px 96 --crop-bottom-px 96 &gt;&gt;%resultFile%</v>
+      </c>
+    </row>
+    <row r="59" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C59">
+        <v>8</v>
+      </c>
+      <c r="D59" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="20"/>
+        <v>8</v>
+      </c>
+      <c r="F59">
+        <f>E59*16</f>
+        <v>128</v>
+      </c>
+      <c r="G59">
+        <f>B$1-F59*2</f>
+        <v>1024</v>
+      </c>
+      <c r="H59">
+        <f>B$2-F59*2</f>
+        <v>464</v>
+      </c>
+      <c r="I59">
+        <f>G59*H59</f>
+        <v>475136</v>
+      </c>
+      <c r="J59">
+        <f>I59*C59/8+54</f>
+        <v>475190</v>
+      </c>
+      <c r="K59">
+        <v>447173</v>
+      </c>
+      <c r="L59" s="1">
+        <f t="shared" si="16"/>
+        <v>0.94104042593488924</v>
+      </c>
+      <c r="N59" t="str">
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop8.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 128 --crop-right-px 128 --crop-top-px 128 --crop-bottom-px 128</v>
+      </c>
+      <c r="O59" t="str">
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop8.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 128 --crop-right-px 128 --crop-top-px 128 --crop-bottom-px 128 &gt;&gt;%resultFile%</v>
+      </c>
+    </row>
+    <row r="60" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C60">
+        <v>8</v>
+      </c>
+      <c r="D60" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="20"/>
+        <v>10</v>
+      </c>
+      <c r="F60">
+        <f>E60*16</f>
+        <v>160</v>
+      </c>
+      <c r="G60">
+        <f>B$1-F60*2</f>
+        <v>960</v>
+      </c>
+      <c r="H60">
+        <f>B$2-F60*2</f>
+        <v>400</v>
+      </c>
+      <c r="I60">
+        <f>G60*H60</f>
+        <v>384000</v>
+      </c>
+      <c r="J60">
+        <f>I60*C60/8+54</f>
+        <v>384054</v>
+      </c>
+      <c r="K60">
+        <v>356312</v>
+      </c>
+      <c r="L60" s="1">
+        <f t="shared" si="16"/>
+        <v>0.92776536632869333</v>
+      </c>
+      <c r="N60" t="str">
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop10.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 160 --crop-right-px 160 --crop-top-px 160 --crop-bottom-px 160</v>
+      </c>
+      <c r="O60" t="str">
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop10.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 160 --crop-right-px 160 --crop-top-px 160 --crop-bottom-px 160 &gt;&gt;%resultFile%</v>
+      </c>
+    </row>
+    <row r="61" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C61">
+        <v>8</v>
+      </c>
+      <c r="D61" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="20"/>
+        <v>12</v>
+      </c>
+      <c r="F61">
+        <f>E61*16</f>
+        <v>192</v>
+      </c>
+      <c r="G61">
+        <f>B$1-F61*2</f>
+        <v>896</v>
+      </c>
+      <c r="H61">
+        <f>B$2-F61*2</f>
+        <v>336</v>
+      </c>
+      <c r="I61">
+        <f>G61*H61</f>
+        <v>301056</v>
+      </c>
+      <c r="J61">
+        <f>I61*C61/8+54</f>
+        <v>301110</v>
+      </c>
+      <c r="K61">
+        <v>277614</v>
+      </c>
+      <c r="L61" s="1">
+        <f t="shared" si="16"/>
+        <v>0.92196871575171868</v>
+      </c>
+      <c r="N61" t="str">
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop12.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 192 --crop-right-px 192 --crop-top-px 192 --crop-bottom-px 192</v>
+      </c>
+      <c r="O61" t="str">
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop12.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 192 --crop-right-px 192 --crop-top-px 192 --crop-bottom-px 192 &gt;&gt;%resultFile%</v>
+      </c>
+    </row>
+    <row r="62" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C62">
+        <v>8</v>
+      </c>
+      <c r="D62" t="s">
+        <v>9</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="20"/>
+        <v>14</v>
+      </c>
+      <c r="F62">
+        <f>E62*16</f>
+        <v>224</v>
+      </c>
+      <c r="G62">
+        <f>B$1-F62*2</f>
+        <v>832</v>
+      </c>
+      <c r="H62">
+        <f>B$2-F62*2</f>
+        <v>272</v>
+      </c>
+      <c r="I62">
+        <f>G62*H62</f>
+        <v>226304</v>
+      </c>
+      <c r="J62">
+        <f>I62*C62/8+54</f>
+        <v>226358</v>
+      </c>
+      <c r="K62">
+        <v>208593</v>
+      </c>
+      <c r="L62" s="1">
+        <f t="shared" si="16"/>
+        <v>0.92151812615414519</v>
+      </c>
+      <c r="N62" t="str">
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop14.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 224 --crop-right-px 224 --crop-top-px 224 --crop-bottom-px 224</v>
+      </c>
+      <c r="O62" t="str">
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop14.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 224 --crop-right-px 224 --crop-top-px 224 --crop-bottom-px 224 &gt;&gt;%resultFile%</v>
+      </c>
+    </row>
+    <row r="63" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C63">
+        <v>8</v>
+      </c>
+      <c r="D63" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="20"/>
+        <v>16</v>
+      </c>
+      <c r="F63">
+        <f>E63*16</f>
+        <v>256</v>
+      </c>
+      <c r="G63">
+        <f>B$1-F63*2</f>
+        <v>768</v>
+      </c>
+      <c r="H63">
+        <f>B$2-F63*2</f>
+        <v>208</v>
+      </c>
+      <c r="I63">
+        <f>G63*H63</f>
+        <v>159744</v>
+      </c>
+      <c r="J63">
+        <f>I63*C63/8+54</f>
+        <v>159798</v>
+      </c>
+      <c r="K63">
+        <v>147198</v>
+      </c>
+      <c r="L63" s="1">
+        <f t="shared" si="16"/>
+        <v>0.9211504524462133</v>
+      </c>
+      <c r="N63" t="str">
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop16.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 256 --crop-right-px 256 --crop-top-px 256 --crop-bottom-px 256</v>
+      </c>
+      <c r="O63" t="str">
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop16.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 256 --crop-right-px 256 --crop-top-px 256 --crop-bottom-px 256 &gt;&gt;%resultFile%</v>
+      </c>
+    </row>
+    <row r="64" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C64">
+        <v>8</v>
+      </c>
+      <c r="D64" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="20"/>
+        <v>18</v>
+      </c>
+      <c r="F64">
+        <f>E64*16</f>
+        <v>288</v>
+      </c>
+      <c r="G64">
+        <f>B$1-F64*2</f>
+        <v>704</v>
+      </c>
+      <c r="H64">
+        <f>B$2-F64*2</f>
+        <v>144</v>
+      </c>
+      <c r="I64">
+        <f>G64*H64</f>
+        <v>101376</v>
+      </c>
+      <c r="J64">
+        <f>I64*C64/8+54</f>
+        <v>101430</v>
+      </c>
+      <c r="K64">
+        <v>92191</v>
+      </c>
+      <c r="L64" s="1">
+        <f t="shared" si="16"/>
+        <v>0.90891255052745734</v>
+      </c>
+      <c r="N64" t="str">
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop18.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 288 --crop-right-px 288 --crop-top-px 288 --crop-bottom-px 288</v>
+      </c>
+      <c r="O64" t="str">
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop18.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 288 --crop-right-px 288 --crop-top-px 288 --crop-bottom-px 288 &gt;&gt;%resultFile%</v>
+      </c>
+    </row>
+    <row r="65" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C65">
+        <v>8</v>
+      </c>
+      <c r="D65" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="20"/>
+        <v>20</v>
+      </c>
+      <c r="F65">
+        <f>E65*16</f>
+        <v>320</v>
+      </c>
+      <c r="G65">
+        <f>B$1-F65*2</f>
+        <v>640</v>
+      </c>
+      <c r="H65">
+        <f>B$2-F65*2</f>
+        <v>80</v>
+      </c>
+      <c r="I65">
+        <f>G65*H65</f>
+        <v>51200</v>
+      </c>
+      <c r="J65">
+        <f>I65*C65/8+54</f>
+        <v>51254</v>
+      </c>
+      <c r="K65">
+        <v>46240</v>
+      </c>
+      <c r="L65" s="1">
+        <f t="shared" si="16"/>
+        <v>0.90217348889842741</v>
+      </c>
+      <c r="N65" t="str">
+        <f t="shared" si="8"/>
+        <v>--destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop20.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 320 --crop-right-px 320 --crop-top-px 320 --crop-bottom-px 320</v>
+      </c>
+      <c r="O65" t="str">
+        <f t="shared" si="9"/>
+        <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop20.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 320 --crop-right-px 320 --crop-top-px 320 --crop-bottom-px 320 &gt;&gt;%resultFile%</v>
+      </c>
+    </row>
+    <row r="66" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C66">
+        <v>8</v>
+      </c>
+      <c r="D66" t="s">
+        <v>9</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="20"/>
         <v>22</v>
       </c>
-      <c r="F42">
-        <f t="shared" si="0"/>
+      <c r="F66">
+        <f>E66*16</f>
         <v>352</v>
       </c>
-      <c r="G42">
-        <f t="shared" si="1"/>
+      <c r="G66">
+        <f>B$1-F66*2</f>
         <v>576</v>
       </c>
-      <c r="H42">
-        <f t="shared" si="2"/>
+      <c r="H66">
+        <f>B$2-F66*2</f>
         <v>16</v>
       </c>
-      <c r="I42">
-        <f t="shared" si="3"/>
+      <c r="I66">
+        <f>G66*H66</f>
         <v>9216</v>
       </c>
-      <c r="J42">
-        <f t="shared" si="4"/>
+      <c r="J66">
+        <f>I66*C66/8+54</f>
         <v>9270</v>
       </c>
-      <c r="K42">
+      <c r="K66">
         <v>8962</v>
       </c>
-      <c r="L42" s="1">
-        <f t="shared" si="5"/>
+      <c r="L66" s="1">
+        <f t="shared" si="16"/>
         <v>0.96677454153182307</v>
       </c>
-      <c r="N42" t="str">
-        <f t="shared" si="6"/>
+      <c r="N66" t="str">
+        <f t="shared" si="8"/>
         <v>--destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop22.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 352 --crop-right-px 352 --crop-top-px 352 --crop-bottom-px 352</v>
       </c>
-      <c r="O42" t="str">
-        <f t="shared" si="7"/>
+      <c r="O66" t="str">
+        <f t="shared" si="9"/>
         <v>dotnet StreamCompress.dll --source-path %resultPath% --source-file-suffix original.bmp --destination-path %resultPath% --destination-file-suffix AsGrayScaleAsHuffmanEncoded-crop22.enc --method AsGrayScaleAsHuffmanEncoded --crop-left-px 352 --crop-right-px 352 --crop-top-px 352 --crop-bottom-px 352 &gt;&gt;%resultFile%</v>
       </c>
     </row>
@@ -2181,4 +4500,581 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8612D509-D5A8-4A5C-96EF-879E8A9BDA07}">
+  <dimension ref="A1:K36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T25" sqref="T25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" customWidth="1"/>
+    <col min="9" max="9" width="26" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1">
+        <v>0.67653154003563154</v>
+      </c>
+      <c r="E1">
+        <v>921654</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.95170747373743292</v>
+      </c>
+      <c r="E2">
+        <v>921654</v>
+      </c>
+      <c r="H2">
+        <v>921654</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0.67653154003563154</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.95170747373743292</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0.75245265576886766</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.75245265576886766</v>
+      </c>
+      <c r="E3">
+        <v>921654</v>
+      </c>
+      <c r="H3">
+        <v>797750</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.69484926355374488</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.95307427138827949</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.77997743654026952</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.69484926355374488</v>
+      </c>
+      <c r="E4">
+        <v>797750</v>
+      </c>
+      <c r="H4">
+        <v>682038</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.70782566367269861</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.95125784780320155</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.76262319694797065</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.95307427138827949</v>
+      </c>
+      <c r="E5">
+        <v>797750</v>
+      </c>
+      <c r="H5">
+        <v>574518</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0.71890697941578852</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.95112076558088698</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0.78602062946678786</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.77997743654026952</v>
+      </c>
+      <c r="E6">
+        <v>797750</v>
+      </c>
+      <c r="H6">
+        <v>475190</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.70919000820724343</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.94104042593488924</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0.79200740756329047</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.70782566367269861</v>
+      </c>
+      <c r="E7">
+        <v>682038</v>
+      </c>
+      <c r="H7">
+        <v>384054</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.68568742937191129</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0.92776536632869333</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0.78869117363704067</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.95125784780320155</v>
+      </c>
+      <c r="E8">
+        <v>682038</v>
+      </c>
+      <c r="H8">
+        <v>301110</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0.67528145860316824</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.92196871575171868</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0.75788582245690939</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.76262319694797065</v>
+      </c>
+      <c r="E9">
+        <v>682038</v>
+      </c>
+      <c r="H9">
+        <v>226358</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0.68024545189478614</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.92151812615414519</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0.7917988319387872</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.71890697941578852</v>
+      </c>
+      <c r="E10">
+        <v>574518</v>
+      </c>
+      <c r="H10">
+        <v>159798</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0.6963478892101278</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.9211504524462133</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0.79124269390105006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.95112076558088698</v>
+      </c>
+      <c r="E11">
+        <v>574518</v>
+      </c>
+      <c r="H11">
+        <v>101430</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0.69023957409050574</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0.90891255052745734</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0.82120674356699197</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.78602062946678786</v>
+      </c>
+      <c r="E12">
+        <v>574518</v>
+      </c>
+      <c r="H12">
+        <v>51254</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0.71098841066063134</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0.90217348889842741</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0.84256838490654384</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.70919000820724343</v>
+      </c>
+      <c r="E13">
+        <v>475190</v>
+      </c>
+      <c r="H13">
+        <v>9270</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0.83193096008629985</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0.96677454153182307</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0.99439050701186626</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.94104042593488924</v>
+      </c>
+      <c r="E14">
+        <v>475190</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.79200740756329047</v>
+      </c>
+      <c r="E15">
+        <v>475190</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.68568742937191129</v>
+      </c>
+      <c r="E16">
+        <v>384054</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.92776536632869333</v>
+      </c>
+      <c r="E17">
+        <v>384054</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.78869117363704067</v>
+      </c>
+      <c r="E18">
+        <v>384054</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.67528145860316824</v>
+      </c>
+      <c r="E19">
+        <v>301110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.92196871575171868</v>
+      </c>
+      <c r="E20">
+        <v>301110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.75788582245690939</v>
+      </c>
+      <c r="E21">
+        <v>301110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.68024545189478614</v>
+      </c>
+      <c r="E22">
+        <v>226358</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.92151812615414519</v>
+      </c>
+      <c r="E23">
+        <v>226358</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.7917988319387872</v>
+      </c>
+      <c r="E24">
+        <v>226358</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.6963478892101278</v>
+      </c>
+      <c r="E25">
+        <v>159798</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.9211504524462133</v>
+      </c>
+      <c r="E26">
+        <v>159798</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0.79124269390105006</v>
+      </c>
+      <c r="E27">
+        <v>159798</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0.69023957409050574</v>
+      </c>
+      <c r="E28">
+        <v>101430</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0.90891255052745734</v>
+      </c>
+      <c r="E29">
+        <v>101430</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0.82120674356699197</v>
+      </c>
+      <c r="E30">
+        <v>101430</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0.71098841066063134</v>
+      </c>
+      <c r="E31">
+        <v>51254</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0.90217348889842741</v>
+      </c>
+      <c r="E32">
+        <v>51254</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0.84256838490654384</v>
+      </c>
+      <c r="E33">
+        <v>51254</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0.83193096008629985</v>
+      </c>
+      <c r="E34">
+        <v>9270</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0.96677454153182307</v>
+      </c>
+      <c r="E35">
+        <v>9270</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0.99439050701186626</v>
+      </c>
+      <c r="E36">
+        <v>9270</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:D36">
+    <sortCondition descending="1" ref="B1:B36"/>
+    <sortCondition ref="A1:A36"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Test coverage report, weekly report
</commit_message>
<xml_diff>
--- a/StreamCompress/CompressionTests.xlsx
+++ b/StreamCompress/CompressionTests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Users\Kalle\Documents\Source\Opiskelu\high-speed-image-stream-compress\StreamCompress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D56D12-9487-4D40-B0C0-56FD5234446C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CA0701-0661-4D3A-8030-4BCFBDC87867}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="17">
   <si>
     <t>Crop</t>
   </si>
@@ -751,7 +751,519 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fi-FI"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Taul1!$J$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AsGZipEncoded</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Taul1!$I$43:$I$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2764854</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2393142</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2046006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1723446</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1425462</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1152054</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>903222</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>678966</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>479286</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>304182</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>153654</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>27702</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Taul1!$J$43:$J$54</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.60172508204773201</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.61867494699436976</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.63217849801026982</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.64637476311993525</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.64131839361554355</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.61416739145908095</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.60070281724758701</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.60103745990226309</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.60584911722854418</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.59905254091300608</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.60483944446613824</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.61158039130748687</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FFE4-4292-B9A8-60C6463A751A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Taul1!$K$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AsLZ78Encoded</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Taul1!$I$43:$I$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2764854</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2393142</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2046006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1723446</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1425462</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1152054</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>903222</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>678966</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>479286</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>304182</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>153654</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>27702</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Taul1!$K$43:$K$54</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.74530807051656256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.76694905693017801</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7884800924337465</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.81724347615184922</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.78369468986195356</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.77946693470965767</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.77807338616641308</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.74514924164096585</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.75822160463689736</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.73720995982668269</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.76719772996472591</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.83856761244675471</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FFE4-4292-B9A8-60C6463A751A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="470271656"/>
+        <c:axId val="470275920"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="470271656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fi-FI"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="470275920"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="470275920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fi-FI"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="470271656"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fi-FI"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fi-FI"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1294,6 +1806,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1327,6 +2342,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1500186</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>33336</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>266699</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Kaavio 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66DE5468-80D5-4E3E-8E15-862F8D1D2FC3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1600,8 +2651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L31" activeCellId="2" sqref="D31:D66 J31:J66 L31:L66"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L7" sqref="L7:L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4504,10 +5555,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8612D509-D5A8-4A5C-96EF-879E8A9BDA07}">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T25" sqref="T25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="W54" sqref="W54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5025,7 +6076,7 @@
         <v>51254</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -5036,7 +6087,7 @@
         <v>51254</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>15</v>
       </c>
@@ -5047,7 +6098,7 @@
         <v>9270</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -5058,7 +6109,7 @@
         <v>9270</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -5069,10 +6120,352 @@
         <v>9270</v>
       </c>
     </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="1">
+        <v>0.60172508204773201</v>
+      </c>
+      <c r="E42">
+        <v>2764854</v>
+      </c>
+      <c r="J42" t="s">
+        <v>16</v>
+      </c>
+      <c r="K42" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" s="1">
+        <v>0.74530807051656256</v>
+      </c>
+      <c r="E43">
+        <v>2393142</v>
+      </c>
+      <c r="I43">
+        <v>2764854</v>
+      </c>
+      <c r="J43" s="1">
+        <v>0.60172508204773201</v>
+      </c>
+      <c r="K43" s="1">
+        <v>0.74530807051656256</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" s="1">
+        <v>0.61867494699436976</v>
+      </c>
+      <c r="E44">
+        <v>2046006</v>
+      </c>
+      <c r="I44">
+        <v>2393142</v>
+      </c>
+      <c r="J44" s="1">
+        <v>0.61867494699436976</v>
+      </c>
+      <c r="K44" s="1">
+        <v>0.76694905693017801</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" s="1">
+        <v>0.76694905693017801</v>
+      </c>
+      <c r="E45">
+        <v>1723446</v>
+      </c>
+      <c r="I45">
+        <v>2046006</v>
+      </c>
+      <c r="J45" s="1">
+        <v>0.63217849801026982</v>
+      </c>
+      <c r="K45" s="1">
+        <v>0.7884800924337465</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D46" s="1">
+        <v>0.63217849801026982</v>
+      </c>
+      <c r="E46">
+        <v>1425462</v>
+      </c>
+      <c r="I46">
+        <v>1723446</v>
+      </c>
+      <c r="J46" s="1">
+        <v>0.64637476311993525</v>
+      </c>
+      <c r="K46" s="1">
+        <v>0.81724347615184922</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47" s="1">
+        <v>0.7884800924337465</v>
+      </c>
+      <c r="E47">
+        <v>1152054</v>
+      </c>
+      <c r="I47">
+        <v>1425462</v>
+      </c>
+      <c r="J47" s="1">
+        <v>0.64131839361554355</v>
+      </c>
+      <c r="K47" s="1">
+        <v>0.78369468986195356</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>16</v>
+      </c>
+      <c r="D48" s="1">
+        <v>0.64637476311993525</v>
+      </c>
+      <c r="E48">
+        <v>903222</v>
+      </c>
+      <c r="I48">
+        <v>1152054</v>
+      </c>
+      <c r="J48" s="1">
+        <v>0.61416739145908095</v>
+      </c>
+      <c r="K48" s="1">
+        <v>0.77946693470965767</v>
+      </c>
+    </row>
+    <row r="49" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49" s="1">
+        <v>0.81724347615184922</v>
+      </c>
+      <c r="E49">
+        <v>678966</v>
+      </c>
+      <c r="I49">
+        <v>903222</v>
+      </c>
+      <c r="J49" s="1">
+        <v>0.60070281724758701</v>
+      </c>
+      <c r="K49" s="1">
+        <v>0.77807338616641308</v>
+      </c>
+    </row>
+    <row r="50" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>16</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0.64131839361554355</v>
+      </c>
+      <c r="E50">
+        <v>479286</v>
+      </c>
+      <c r="I50">
+        <v>678966</v>
+      </c>
+      <c r="J50" s="1">
+        <v>0.60103745990226309</v>
+      </c>
+      <c r="K50" s="1">
+        <v>0.74514924164096585</v>
+      </c>
+    </row>
+    <row r="51" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" s="1">
+        <v>0.78369468986195356</v>
+      </c>
+      <c r="E51">
+        <v>304182</v>
+      </c>
+      <c r="I51">
+        <v>479286</v>
+      </c>
+      <c r="J51" s="1">
+        <v>0.60584911722854418</v>
+      </c>
+      <c r="K51" s="1">
+        <v>0.75822160463689736</v>
+      </c>
+    </row>
+    <row r="52" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>16</v>
+      </c>
+      <c r="D52" s="1">
+        <v>0.61416739145908095</v>
+      </c>
+      <c r="E52">
+        <v>153654</v>
+      </c>
+      <c r="I52">
+        <v>304182</v>
+      </c>
+      <c r="J52" s="1">
+        <v>0.59905254091300608</v>
+      </c>
+      <c r="K52" s="1">
+        <v>0.73720995982668269</v>
+      </c>
+    </row>
+    <row r="53" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0.77946693470965767</v>
+      </c>
+      <c r="E53">
+        <v>27702</v>
+      </c>
+      <c r="I53">
+        <v>153654</v>
+      </c>
+      <c r="J53" s="1">
+        <v>0.60483944446613824</v>
+      </c>
+      <c r="K53" s="1">
+        <v>0.76719772996472591</v>
+      </c>
+    </row>
+    <row r="54" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>16</v>
+      </c>
+      <c r="D54" s="1">
+        <v>0.60070281724758701</v>
+      </c>
+      <c r="I54">
+        <v>27702</v>
+      </c>
+      <c r="J54" s="1">
+        <v>0.61158039130748687</v>
+      </c>
+      <c r="K54" s="1">
+        <v>0.83856761244675471</v>
+      </c>
+    </row>
+    <row r="55" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>2</v>
+      </c>
+      <c r="D55" s="1">
+        <v>0.77807338616641308</v>
+      </c>
+    </row>
+    <row r="56" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>16</v>
+      </c>
+      <c r="D56" s="1">
+        <v>0.60103745990226309</v>
+      </c>
+    </row>
+    <row r="57" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>2</v>
+      </c>
+      <c r="D57" s="1">
+        <v>0.74514924164096585</v>
+      </c>
+    </row>
+    <row r="58" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>16</v>
+      </c>
+      <c r="D58" s="1">
+        <v>0.60584911722854418</v>
+      </c>
+    </row>
+    <row r="59" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>2</v>
+      </c>
+      <c r="D59" s="1">
+        <v>0.75822160463689736</v>
+      </c>
+    </row>
+    <row r="60" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>16</v>
+      </c>
+      <c r="D60" s="1">
+        <v>0.59905254091300608</v>
+      </c>
+    </row>
+    <row r="61" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>2</v>
+      </c>
+      <c r="D61" s="1">
+        <v>0.73720995982668269</v>
+      </c>
+    </row>
+    <row r="62" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>16</v>
+      </c>
+      <c r="D62" s="1">
+        <v>0.60483944446613824</v>
+      </c>
+    </row>
+    <row r="63" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>2</v>
+      </c>
+      <c r="D63" s="1">
+        <v>0.76719772996472591</v>
+      </c>
+    </row>
+    <row r="64" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>16</v>
+      </c>
+      <c r="D64" s="1">
+        <v>0.61158039130748687</v>
+      </c>
+    </row>
+    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>2</v>
+      </c>
+      <c r="D65" s="1">
+        <v>0.83856761244675471</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:D36">
-    <sortCondition descending="1" ref="B1:B36"/>
-    <sortCondition ref="A1:A36"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C42:E65">
+    <sortCondition descending="1" ref="E42:E65"/>
+    <sortCondition ref="C42:C65"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>